<commit_message>
CRUD Operations completed on admin part
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX23"/>
+  <dimension ref="A1:AX24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -542,102 +542,102 @@
         <v>isTrending</v>
       </c>
       <c r="AU1" t="str">
+        <v>image_url</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>date_modified</v>
+      </c>
+      <c r="AW1" t="str">
         <v>ID</v>
       </c>
-      <c r="AV1" t="str">
+      <c r="AX1" t="str">
         <v>date_created</v>
-      </c>
-      <c r="AW1" t="str">
-        <v>date_modified</v>
-      </c>
-      <c r="AX1" t="str">
-        <v>image_url</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="str">
-        <v>Johnnie Walker Blue Label</v>
+        <v>Dom Pérignon Vintage Champagne2</v>
       </c>
       <c r="D2" t="str">
-        <v>Johnnie Walker Blue Label</v>
+        <v>Dom Pérignon Vintage Champagne2</v>
       </c>
       <c r="E2" t="str">
-        <v>A remarkable blend made up of the finest aged Scottish whiskies with a depth of flavor that's truly extraordinary.</v>
+        <v>Elegant and luxurious, Dom Pérignon is a testament to the finest in champagne making, with vibrant notes of almond, citrus, and toasted brioche.</v>
       </c>
       <c r="F2" t="str">
-        <v>spirits</v>
+        <v>wine</v>
       </c>
       <c r="G2" t="str">
-        <v>SPIRITS</v>
+        <v>WINE</v>
       </c>
       <c r="H2" t="str">
-        <v>whiskey</v>
+        <v>champagne</v>
       </c>
       <c r="I2" t="str">
-        <v>WHISKEY</v>
+        <v>CHAMPAGNE</v>
       </c>
       <c r="J2" t="str">
-        <v xml:space="preserve">WHISKEY  </v>
+        <v xml:space="preserve">CHAMPAGNE  </v>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>Champagne Blend</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>CHAMPAGNE BLEND</v>
       </c>
       <c r="M2" t="str">
-        <v>Johnnie Walker</v>
+        <v>Dom Pérignon</v>
       </c>
       <c r="N2" t="str">
-        <v>JOHNNIE WALKER</v>
+        <v>DOM PÉRIGNON</v>
       </c>
       <c r="O2" t="str">
-        <v>Scotland</v>
+        <v>France</v>
       </c>
       <c r="P2" t="str">
-        <v>SCOTLAND</v>
+        <v>FRANCE</v>
       </c>
       <c r="Q2" t="str">
-        <v>Highlands</v>
+        <v>Champagne</v>
       </c>
       <c r="R2">
-        <v>249.99</v>
+        <v>219.98</v>
       </c>
       <c r="S2">
-        <v>199.99</v>
+        <v>175.95</v>
       </c>
       <c r="T2">
-        <v>249.99</v>
+        <v>219.98</v>
       </c>
       <c r="U2" t="str">
-        <v>https://ext.same-assets.com/1701767421/458812689.png</v>
+        <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="V2" t="str">
-        <v>https://ext.same-assets.com/1701767421/458812689.png</v>
+        <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="W2" t="str">
-        <v>A remarkable blend made up of the finest aged Scottish whiskies with a depth of flavor that's truly extraordinary.</v>
-      </c>
-      <c r="X2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="str">
-        <v>40%</v>
+        <v>Elegant and luxurious, Dom Pérignon is a testament to the finest in champagne making, with vibrant notes of almond, citrus, and toasted brioche.</v>
+      </c>
+      <c r="X2" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y2" t="str">
+        <v>true</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>true</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>true</v>
+      </c>
+      <c r="AB2">
+        <v>12.5</v>
       </c>
       <c r="AC2" t="str">
         <v>750ml</v>
@@ -649,13 +649,13 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF2" t="str">
-        <v>SPIRITS | WHISKEY</v>
+        <v>WINE | CHAMPAGNE</v>
       </c>
       <c r="AG2" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH2">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AI2" t="str">
         <v>featured</v>
@@ -688,96 +688,102 @@
         <v>open</v>
       </c>
       <c r="AS2" t="str">
-        <v/>
-      </c>
-      <c r="AT2" t="b">
-        <v>0</v>
+        <v>WHITE</v>
+      </c>
+      <c r="AT2" t="str">
+        <v>true</v>
+      </c>
+      <c r="AU2" t="str">
+        <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
+      </c>
+      <c r="AV2" t="str">
+        <v>2025-03-29T02:10:07.293Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="str">
-        <v>Dom Pérignon Vintage Champagne</v>
+        <v>Macallan Rare Cask Single Malt</v>
       </c>
       <c r="D3" t="str">
-        <v>Dom Pérignon Vintage Champagne</v>
+        <v>Macallan Rare Cask Single Malt</v>
       </c>
       <c r="E3" t="str">
-        <v>Elegant and luxurious, Dom Pérignon is a testament to the finest in champagne making, with vibrant notes of almond, citrus, and toasted brioche.</v>
+        <v>Drawn from the broadest spectrum of casks, Rare Cask showcases the diversity of oak types and sizes that The Macallan uses to mature its whisky.</v>
       </c>
       <c r="F3" t="str">
-        <v>wine</v>
+        <v>spirits</v>
       </c>
       <c r="G3" t="str">
-        <v>WINE</v>
+        <v>SPIRITS</v>
       </c>
       <c r="H3" t="str">
-        <v>champagne</v>
+        <v>scotch</v>
       </c>
       <c r="I3" t="str">
-        <v>CHAMPAGNE</v>
+        <v>SCOTCH</v>
       </c>
       <c r="J3" t="str">
-        <v xml:space="preserve">CHAMPAGNE  </v>
+        <v xml:space="preserve">SCOTCH  </v>
       </c>
       <c r="K3" t="str">
-        <v>Champagne Blend</v>
+        <v/>
       </c>
       <c r="L3" t="str">
-        <v>CHAMPAGNE BLEND</v>
+        <v/>
       </c>
       <c r="M3" t="str">
-        <v>Dom Pérignon</v>
+        <v>The Macallan</v>
       </c>
       <c r="N3" t="str">
-        <v>DOM PÉRIGNON</v>
+        <v>THE MACALLAN</v>
       </c>
       <c r="O3" t="str">
-        <v>France</v>
+        <v>Scotland</v>
       </c>
       <c r="P3" t="str">
-        <v>FRANCE</v>
+        <v>SCOTLAND</v>
       </c>
       <c r="Q3" t="str">
-        <v>Champagne</v>
+        <v>Speyside</v>
       </c>
       <c r="R3">
-        <v>219.95</v>
+        <v>299.66</v>
       </c>
       <c r="S3">
-        <v>175.95</v>
+        <v>239.99</v>
       </c>
       <c r="T3">
-        <v>219.95</v>
+        <v>299.66</v>
       </c>
       <c r="U3" t="str">
-        <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
+        <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
       </c>
       <c r="V3" t="str">
-        <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
+        <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
       </c>
       <c r="W3" t="str">
-        <v>Elegant and luxurious, Dom Pérignon is a testament to the finest in champagne making, with vibrant notes of almond, citrus, and toasted brioche.</v>
-      </c>
-      <c r="X3" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="str">
-        <v>12.5%</v>
+        <v>Drawn from the broadest spectrum of casks, Rare Cask showcases the diversity of oak types and sizes that The Macallan uses to mature its whisky.</v>
+      </c>
+      <c r="X3" t="str">
+        <v>true</v>
+      </c>
+      <c r="Y3" t="str">
+        <v>true</v>
+      </c>
+      <c r="Z3" t="str">
+        <v>true</v>
+      </c>
+      <c r="AA3" t="str">
+        <v>true</v>
+      </c>
+      <c r="AB3">
+        <v>43</v>
       </c>
       <c r="AC3" t="str">
         <v>750ml</v>
@@ -789,13 +795,13 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF3" t="str">
-        <v>WINE | CHAMPAGNE</v>
+        <v>SPIRITS | SCOTCH</v>
       </c>
       <c r="AG3" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI3" t="str">
         <v>featured</v>
@@ -828,96 +834,102 @@
         <v>open</v>
       </c>
       <c r="AS3" t="str">
-        <v>WHITE</v>
-      </c>
-      <c r="AT3" t="b">
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="AT3" t="str">
+        <v>true</v>
+      </c>
+      <c r="AU3" t="str">
+        <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
+      </c>
+      <c r="AV3" t="str">
+        <v>2025-03-28T15:21:02.207Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="str">
-        <v>Macallan Rare Cask Single Malt</v>
+        <v>Veuve Clicquot Yellow Label Brut</v>
       </c>
       <c r="D4" t="str">
-        <v>Macallan Rare Cask Single Malt</v>
+        <v>Veuve Clicquot Yellow Label Brut</v>
       </c>
       <c r="E4" t="str">
-        <v>Drawn from the broadest spectrum of casks, Rare Cask showcases the diversity of oak types and sizes that The Macallan uses to mature its whisky.</v>
+        <v>A perfect balance of power and finesse with crisp fruity flavors and a silky mouthfeel that distinguishes Yellow Label from other champagnes.</v>
       </c>
       <c r="F4" t="str">
-        <v>spirits</v>
+        <v>wine</v>
       </c>
       <c r="G4" t="str">
-        <v>SPIRITS</v>
+        <v>WINE</v>
       </c>
       <c r="H4" t="str">
-        <v>scotch</v>
+        <v>champagne</v>
       </c>
       <c r="I4" t="str">
-        <v>SCOTCH</v>
+        <v>CHAMPAGNE</v>
       </c>
       <c r="J4" t="str">
-        <v xml:space="preserve">SCOTCH  </v>
+        <v xml:space="preserve">CHAMPAGNE  </v>
       </c>
       <c r="K4" t="str">
-        <v/>
+        <v>Champagne Blend</v>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>CHAMPAGNE BLEND</v>
       </c>
       <c r="M4" t="str">
-        <v>The Macallan</v>
+        <v>Veuve Clicquot</v>
       </c>
       <c r="N4" t="str">
-        <v>THE MACALLAN</v>
+        <v>VEUVE CLICQUOT</v>
       </c>
       <c r="O4" t="str">
-        <v>Scotland</v>
+        <v>France</v>
       </c>
       <c r="P4" t="str">
-        <v>SCOTLAND</v>
+        <v>FRANCE</v>
       </c>
       <c r="Q4" t="str">
-        <v>Speyside</v>
+        <v>Champagne</v>
       </c>
       <c r="R4">
-        <v>299.99</v>
+        <v>69.95</v>
       </c>
       <c r="S4">
-        <v>239.99</v>
+        <v>55.96</v>
       </c>
       <c r="T4">
-        <v>299.99</v>
+        <v>69.95</v>
       </c>
       <c r="U4" t="str">
-        <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
+        <v>https://ext.same-assets.com/0/2034363354.svg</v>
       </c>
       <c r="V4" t="str">
-        <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
+        <v>https://ext.same-assets.com/0/2034363354.svg</v>
       </c>
       <c r="W4" t="str">
-        <v>Drawn from the broadest spectrum of casks, Rare Cask showcases the diversity of oak types and sizes that The Macallan uses to mature its whisky.</v>
+        <v>A perfect balance of power and finesse with crisp fruity flavors and a silky mouthfeel that distinguishes Yellow Label from other champagnes.</v>
       </c>
       <c r="X4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="b">
         <v>1</v>
       </c>
       <c r="AB4" t="str">
-        <v>43%</v>
+        <v>12%</v>
       </c>
       <c r="AC4" t="str">
         <v>750ml</v>
@@ -929,13 +941,13 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF4" t="str">
-        <v>SPIRITS | SCOTCH</v>
+        <v>WINE | CHAMPAGNE</v>
       </c>
       <c r="AG4" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AI4" t="str">
         <v>featured</v>
@@ -968,54 +980,54 @@
         <v>open</v>
       </c>
       <c r="AS4" t="str">
-        <v/>
+        <v>WHITE</v>
       </c>
       <c r="AT4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="str">
-        <v>Veuve Clicquot Yellow Label Brut</v>
+        <v>Grey Goose Vodka</v>
       </c>
       <c r="D5" t="str">
-        <v>Veuve Clicquot Yellow Label Brut</v>
+        <v>Grey Goose Vodka</v>
       </c>
       <c r="E5" t="str">
-        <v>A perfect balance of power and finesse with crisp fruity flavors and a silky mouthfeel that distinguishes Yellow Label from other champagnes.</v>
+        <v>Created with the finest French ingredients, Grey Goose is a premium vodka with a smooth, exceptional taste that's perfect for cocktails or on the rocks.</v>
       </c>
       <c r="F5" t="str">
-        <v>wine</v>
+        <v>spirits</v>
       </c>
       <c r="G5" t="str">
-        <v>WINE</v>
+        <v>SPIRITS</v>
       </c>
       <c r="H5" t="str">
-        <v>champagne</v>
+        <v>vodka</v>
       </c>
       <c r="I5" t="str">
-        <v>CHAMPAGNE</v>
+        <v>VODKA</v>
       </c>
       <c r="J5" t="str">
-        <v xml:space="preserve">CHAMPAGNE  </v>
+        <v xml:space="preserve">VODKA  </v>
       </c>
       <c r="K5" t="str">
-        <v>Champagne Blend</v>
+        <v/>
       </c>
       <c r="L5" t="str">
-        <v>CHAMPAGNE BLEND</v>
+        <v/>
       </c>
       <c r="M5" t="str">
-        <v>Veuve Clicquot</v>
+        <v>Grey Goose</v>
       </c>
       <c r="N5" t="str">
-        <v>VEUVE CLICQUOT</v>
+        <v>GREY GOOSE</v>
       </c>
       <c r="O5" t="str">
         <v>France</v>
@@ -1024,25 +1036,25 @@
         <v>FRANCE</v>
       </c>
       <c r="Q5" t="str">
-        <v>Champagne</v>
+        <v/>
       </c>
       <c r="R5">
-        <v>69.95</v>
+        <v>45.99</v>
       </c>
       <c r="S5">
-        <v>55.96</v>
+        <v>36.79</v>
       </c>
       <c r="T5">
-        <v>69.95</v>
+        <v>45.99</v>
       </c>
       <c r="U5" t="str">
-        <v>https://ext.same-assets.com/0/2034363354.svg</v>
+        <v>https://ext.same-assets.com/0/2637691418.svg</v>
       </c>
       <c r="V5" t="str">
-        <v>https://ext.same-assets.com/0/2034363354.svg</v>
+        <v>https://ext.same-assets.com/0/2637691418.svg</v>
       </c>
       <c r="W5" t="str">
-        <v>A perfect balance of power and finesse with crisp fruity flavors and a silky mouthfeel that distinguishes Yellow Label from other champagnes.</v>
+        <v>Created with the finest French ingredients, Grey Goose is a premium vodka with a smooth, exceptional taste that's perfect for cocktails or on the rocks.</v>
       </c>
       <c r="X5" t="b">
         <v>0</v>
@@ -1054,10 +1066,10 @@
         <v>0</v>
       </c>
       <c r="AA5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="str">
-        <v>12%</v>
+        <v>40%</v>
       </c>
       <c r="AC5" t="str">
         <v>750ml</v>
@@ -1069,16 +1081,16 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF5" t="str">
-        <v>WINE | CHAMPAGNE</v>
+        <v>SPIRITS | VODKA</v>
       </c>
       <c r="AG5" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AI5" t="str">
-        <v>featured</v>
+        <v>visible</v>
       </c>
       <c r="AJ5" t="str">
         <v>simple</v>
@@ -1108,27 +1120,27 @@
         <v>open</v>
       </c>
       <c r="AS5" t="str">
-        <v>WHITE</v>
+        <v/>
       </c>
       <c r="AT5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="str">
-        <v>Grey Goose Vodka</v>
+        <v>Don Julio 1942 Tequila</v>
       </c>
       <c r="D6" t="str">
-        <v>Grey Goose Vodka</v>
+        <v>Don Julio 1942 Tequila</v>
       </c>
       <c r="E6" t="str">
-        <v>Created with the finest French ingredients, Grey Goose is a premium vodka with a smooth, exceptional taste that's perfect for cocktails or on the rocks.</v>
+        <v>A luxurious añejo tequila aged for a minimum of two and a half years. Rich caramel and chocolate notes with hints of vanilla and roasted agave.</v>
       </c>
       <c r="F6" t="str">
         <v>spirits</v>
@@ -1137,13 +1149,13 @@
         <v>SPIRITS</v>
       </c>
       <c r="H6" t="str">
-        <v>vodka</v>
+        <v>tequila</v>
       </c>
       <c r="I6" t="str">
-        <v>VODKA</v>
+        <v>TEQUILA</v>
       </c>
       <c r="J6" t="str">
-        <v xml:space="preserve">VODKA  </v>
+        <v xml:space="preserve">TEQUILA  </v>
       </c>
       <c r="K6" t="str">
         <v/>
@@ -1152,49 +1164,49 @@
         <v/>
       </c>
       <c r="M6" t="str">
-        <v>Grey Goose</v>
+        <v>Don Julio</v>
       </c>
       <c r="N6" t="str">
-        <v>GREY GOOSE</v>
+        <v>DON JULIO</v>
       </c>
       <c r="O6" t="str">
-        <v>France</v>
+        <v>Mexico</v>
       </c>
       <c r="P6" t="str">
-        <v>FRANCE</v>
+        <v>MEXICO</v>
       </c>
       <c r="Q6" t="str">
-        <v/>
+        <v>Jalisco</v>
       </c>
       <c r="R6">
-        <v>45.99</v>
+        <v>199.99</v>
       </c>
       <c r="S6">
-        <v>36.79</v>
+        <v>159.99</v>
       </c>
       <c r="T6">
-        <v>45.99</v>
+        <v>199.99</v>
       </c>
       <c r="U6" t="str">
-        <v>https://ext.same-assets.com/0/2637691418.svg</v>
+        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/820584-1-300x300.jpg</v>
       </c>
       <c r="V6" t="str">
-        <v>https://ext.same-assets.com/0/2637691418.svg</v>
+        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/820584-1-300x300.jpg</v>
       </c>
       <c r="W6" t="str">
-        <v>Created with the finest French ingredients, Grey Goose is a premium vodka with a smooth, exceptional taste that's perfect for cocktails or on the rocks.</v>
+        <v>A luxurious añejo tequila aged for a minimum of two and a half years. Rich caramel and chocolate notes with hints of vanilla and roasted agave.</v>
       </c>
       <c r="X6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" t="str">
         <v>40%</v>
@@ -1209,16 +1221,16 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF6" t="str">
-        <v>SPIRITS | VODKA</v>
+        <v>SPIRITS | TEQUILA</v>
       </c>
       <c r="AG6" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AI6" t="str">
-        <v>visible</v>
+        <v>featured</v>
       </c>
       <c r="AJ6" t="str">
         <v>simple</v>
@@ -1251,24 +1263,24 @@
         <v/>
       </c>
       <c r="AT6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>599</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>599</v>
       </c>
       <c r="C7" t="str">
-        <v>Don Julio 1942 Tequila</v>
+        <v>Macallan 18 Year Double Cask</v>
       </c>
       <c r="D7" t="str">
-        <v>Don Julio 1942 Tequila</v>
+        <v>Macallan 18 Year Double Cask</v>
       </c>
       <c r="E7" t="str">
-        <v>A luxurious añejo tequila aged for a minimum of two and a half years. Rich caramel and chocolate notes with hints of vanilla and roasted agave.</v>
+        <v>A sophisticated single malt matured in both American and European oak sherry seasoned casks. Notes of dried fruits, ginger and toffee with a rich oak finish.</v>
       </c>
       <c r="F7" t="str">
         <v>spirits</v>
@@ -1277,13 +1289,13 @@
         <v>SPIRITS</v>
       </c>
       <c r="H7" t="str">
-        <v>tequila</v>
+        <v>scotch</v>
       </c>
       <c r="I7" t="str">
-        <v>TEQUILA</v>
+        <v>SCOTCH</v>
       </c>
       <c r="J7" t="str">
-        <v xml:space="preserve">TEQUILA  </v>
+        <v xml:space="preserve">SCOTCH  </v>
       </c>
       <c r="K7" t="str">
         <v/>
@@ -1292,37 +1304,37 @@
         <v/>
       </c>
       <c r="M7" t="str">
-        <v>Don Julio</v>
+        <v>The Macallan</v>
       </c>
       <c r="N7" t="str">
-        <v>DON JULIO</v>
+        <v>THE MACALLAN</v>
       </c>
       <c r="O7" t="str">
-        <v>Mexico</v>
+        <v>Scotland</v>
       </c>
       <c r="P7" t="str">
-        <v>MEXICO</v>
+        <v>SCOTLAND</v>
       </c>
       <c r="Q7" t="str">
-        <v>Jalisco</v>
+        <v>Speyside</v>
       </c>
       <c r="R7">
-        <v>199.99</v>
+        <v>349.99</v>
       </c>
       <c r="S7">
-        <v>159.99</v>
+        <v>279.99</v>
       </c>
       <c r="T7">
-        <v>199.99</v>
+        <v>349.99</v>
       </c>
       <c r="U7" t="str">
-        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/820584-1-300x300.jpg</v>
+        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/812636-1-300x300.jpg</v>
       </c>
       <c r="V7" t="str">
-        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/820584-1-300x300.jpg</v>
+        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/812636-1-300x300.jpg</v>
       </c>
       <c r="W7" t="str">
-        <v>A luxurious añejo tequila aged for a minimum of two and a half years. Rich caramel and chocolate notes with hints of vanilla and roasted agave.</v>
+        <v>A sophisticated single malt matured in both American and European oak sherry seasoned casks. Notes of dried fruits, ginger and toffee with a rich oak finish.</v>
       </c>
       <c r="X7" t="b">
         <v>1</v>
@@ -1337,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="AB7" t="str">
-        <v>40%</v>
+        <v>43%</v>
       </c>
       <c r="AC7" t="str">
         <v>750ml</v>
@@ -1349,13 +1361,13 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF7" t="str">
-        <v>SPIRITS | TEQUILA</v>
+        <v>SPIRITS | SCOTCH</v>
       </c>
       <c r="AG7" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI7" t="str">
         <v>featured</v>
@@ -1391,24 +1403,24 @@
         <v/>
       </c>
       <c r="AT7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>599</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>599</v>
+        <v>7</v>
       </c>
       <c r="C8" t="str">
-        <v>Macallan 18 Year Double Cask</v>
+        <v>Hendrick's Gin</v>
       </c>
       <c r="D8" t="str">
-        <v>Macallan 18 Year Double Cask</v>
+        <v>Hendrick's Gin</v>
       </c>
       <c r="E8" t="str">
-        <v>A sophisticated single malt matured in both American and European oak sherry seasoned casks. Notes of dried fruits, ginger and toffee with a rich oak finish.</v>
+        <v>A most unusual gin infused with rose and cucumber, offering a delightfully floral aroma with a crisp finish.</v>
       </c>
       <c r="F8" t="str">
         <v>spirits</v>
@@ -1417,13 +1429,13 @@
         <v>SPIRITS</v>
       </c>
       <c r="H8" t="str">
-        <v>scotch</v>
+        <v>gin</v>
       </c>
       <c r="I8" t="str">
-        <v>SCOTCH</v>
+        <v>GIN</v>
       </c>
       <c r="J8" t="str">
-        <v xml:space="preserve">SCOTCH  </v>
+        <v xml:space="preserve">GIN  </v>
       </c>
       <c r="K8" t="str">
         <v/>
@@ -1432,10 +1444,10 @@
         <v/>
       </c>
       <c r="M8" t="str">
-        <v>The Macallan</v>
+        <v>Hendrick's</v>
       </c>
       <c r="N8" t="str">
-        <v>THE MACALLAN</v>
+        <v>HENDRICK'S</v>
       </c>
       <c r="O8" t="str">
         <v>Scotland</v>
@@ -1444,40 +1456,40 @@
         <v>SCOTLAND</v>
       </c>
       <c r="Q8" t="str">
-        <v>Speyside</v>
+        <v/>
       </c>
       <c r="R8">
-        <v>349.99</v>
+        <v>39.99</v>
       </c>
       <c r="S8">
-        <v>279.99</v>
+        <v>31.99</v>
       </c>
       <c r="T8">
-        <v>349.99</v>
+        <v>39.99</v>
       </c>
       <c r="U8" t="str">
-        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/812636-1-300x300.jpg</v>
+        <v>https://ext.same-assets.com/1701767421/3124449398.gif</v>
       </c>
       <c r="V8" t="str">
-        <v>https://orders.demo.liquoronline.ca/wp-content/uploads/2023/09/812636-1-300x300.jpg</v>
+        <v>https://ext.same-assets.com/1701767421/3124449398.gif</v>
       </c>
       <c r="W8" t="str">
-        <v>A sophisticated single malt matured in both American and European oak sherry seasoned casks. Notes of dried fruits, ginger and toffee with a rich oak finish.</v>
+        <v>A most unusual gin infused with rose and cucumber, offering a delightfully floral aroma with a crisp finish.</v>
       </c>
       <c r="X8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="b">
         <v>1</v>
       </c>
       <c r="AB8" t="str">
-        <v>43%</v>
+        <v>44%</v>
       </c>
       <c r="AC8" t="str">
         <v>750ml</v>
@@ -1489,13 +1501,13 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF8" t="str">
-        <v>SPIRITS | SCOTCH</v>
+        <v>SPIRITS | GIN</v>
       </c>
       <c r="AG8" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH8">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="AI8" t="str">
         <v>featured</v>
@@ -1531,24 +1543,24 @@
         <v/>
       </c>
       <c r="AT8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="str">
-        <v>Hendrick's Gin</v>
+        <v>Jack Daniel's Old No. 7</v>
       </c>
       <c r="D9" t="str">
-        <v>Hendrick's Gin</v>
+        <v>Jack Daniel's Old No. 7</v>
       </c>
       <c r="E9" t="str">
-        <v>A most unusual gin infused with rose and cucumber, offering a delightfully floral aroma with a crisp finish.</v>
+        <v>Charcoal mellowed, drop by drop, then matured in handcrafted barrels. It's this unique process that gives Jack Daniel's its rare smoothness.</v>
       </c>
       <c r="F9" t="str">
         <v>spirits</v>
@@ -1557,13 +1569,13 @@
         <v>SPIRITS</v>
       </c>
       <c r="H9" t="str">
-        <v>gin</v>
+        <v>whiskey</v>
       </c>
       <c r="I9" t="str">
-        <v>GIN</v>
+        <v>WHISKEY</v>
       </c>
       <c r="J9" t="str">
-        <v xml:space="preserve">GIN  </v>
+        <v xml:space="preserve">WHISKEY  </v>
       </c>
       <c r="K9" t="str">
         <v/>
@@ -1572,37 +1584,37 @@
         <v/>
       </c>
       <c r="M9" t="str">
-        <v>Hendrick's</v>
+        <v>Jack Daniel's</v>
       </c>
       <c r="N9" t="str">
-        <v>HENDRICK'S</v>
+        <v>JACK DANIEL'S</v>
       </c>
       <c r="O9" t="str">
-        <v>Scotland</v>
+        <v>United States</v>
       </c>
       <c r="P9" t="str">
-        <v>SCOTLAND</v>
+        <v>UNITED STATES</v>
       </c>
       <c r="Q9" t="str">
-        <v/>
+        <v>Tennessee</v>
       </c>
       <c r="R9">
-        <v>39.99</v>
+        <v>29.99</v>
       </c>
       <c r="S9">
-        <v>31.99</v>
+        <v>23.99</v>
       </c>
       <c r="T9">
-        <v>39.99</v>
+        <v>29.99</v>
       </c>
       <c r="U9" t="str">
-        <v>https://ext.same-assets.com/1701767421/3124449398.gif</v>
+        <v>https://ext.same-assets.com/1701767421/1810180129.png</v>
       </c>
       <c r="V9" t="str">
-        <v>https://ext.same-assets.com/1701767421/3124449398.gif</v>
+        <v>https://ext.same-assets.com/1701767421/1810180129.png</v>
       </c>
       <c r="W9" t="str">
-        <v>A most unusual gin infused with rose and cucumber, offering a delightfully floral aroma with a crisp finish.</v>
+        <v>Charcoal mellowed, drop by drop, then matured in handcrafted barrels. It's this unique process that gives Jack Daniel's its rare smoothness.</v>
       </c>
       <c r="X9" t="b">
         <v>0</v>
@@ -1614,10 +1626,10 @@
         <v>0</v>
       </c>
       <c r="AA9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="str">
-        <v>44%</v>
+        <v>40%</v>
       </c>
       <c r="AC9" t="str">
         <v>750ml</v>
@@ -1629,16 +1641,16 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF9" t="str">
-        <v>SPIRITS | GIN</v>
+        <v>SPIRITS | WHISKEY</v>
       </c>
       <c r="AG9" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AI9" t="str">
-        <v>featured</v>
+        <v>visible</v>
       </c>
       <c r="AJ9" t="str">
         <v>simple</v>
@@ -1671,51 +1683,51 @@
         <v/>
       </c>
       <c r="AT9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" t="str">
-        <v>Jack Daniel's Old No. 7</v>
+        <v>Caymus Cabernet Sauvignon</v>
       </c>
       <c r="D10" t="str">
-        <v>Jack Daniel's Old No. 7</v>
+        <v>Caymus Cabernet Sauvignon</v>
       </c>
       <c r="E10" t="str">
-        <v>Charcoal mellowed, drop by drop, then matured in handcrafted barrels. It's this unique process that gives Jack Daniel's its rare smoothness.</v>
+        <v>A rich, deeply colored and concentrated Cabernet from Napa Valley with scents of dark berries, currants and sweet vanilla oak.</v>
       </c>
       <c r="F10" t="str">
-        <v>spirits</v>
+        <v>wine</v>
       </c>
       <c r="G10" t="str">
-        <v>SPIRITS</v>
+        <v>WINE</v>
       </c>
       <c r="H10" t="str">
-        <v>whiskey</v>
+        <v>red</v>
       </c>
       <c r="I10" t="str">
-        <v>WHISKEY</v>
+        <v>RED</v>
       </c>
       <c r="J10" t="str">
-        <v xml:space="preserve">WHISKEY  </v>
+        <v xml:space="preserve">RED  </v>
       </c>
       <c r="K10" t="str">
-        <v/>
+        <v>Cabernet Sauvignon</v>
       </c>
       <c r="L10" t="str">
-        <v/>
+        <v>CABERNET SAUVIGNON</v>
       </c>
       <c r="M10" t="str">
-        <v>Jack Daniel's</v>
+        <v>Caymus Vineyards</v>
       </c>
       <c r="N10" t="str">
-        <v>JACK DANIEL'S</v>
+        <v>CAYMUS VINEYARDS</v>
       </c>
       <c r="O10" t="str">
         <v>United States</v>
@@ -1724,25 +1736,25 @@
         <v>UNITED STATES</v>
       </c>
       <c r="Q10" t="str">
-        <v>Tennessee</v>
+        <v>Napa Valley</v>
       </c>
       <c r="R10">
-        <v>29.99</v>
+        <v>89.95</v>
       </c>
       <c r="S10">
-        <v>23.99</v>
+        <v>71.96</v>
       </c>
       <c r="T10">
-        <v>29.99</v>
+        <v>89.95</v>
       </c>
       <c r="U10" t="str">
-        <v>https://ext.same-assets.com/1701767421/1810180129.png</v>
+        <v>https://ext.same-assets.com/1701767421/4224202088.png</v>
       </c>
       <c r="V10" t="str">
-        <v>https://ext.same-assets.com/1701767421/1810180129.png</v>
+        <v>https://ext.same-assets.com/1701767421/4224202088.png</v>
       </c>
       <c r="W10" t="str">
-        <v>Charcoal mellowed, drop by drop, then matured in handcrafted barrels. It's this unique process that gives Jack Daniel's its rare smoothness.</v>
+        <v>A rich, deeply colored and concentrated Cabernet from Napa Valley with scents of dark berries, currants and sweet vanilla oak.</v>
       </c>
       <c r="X10" t="b">
         <v>0</v>
@@ -1754,10 +1766,10 @@
         <v>0</v>
       </c>
       <c r="AA10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10" t="str">
-        <v>40%</v>
+        <v>14.6%</v>
       </c>
       <c r="AC10" t="str">
         <v>750ml</v>
@@ -1769,16 +1781,16 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF10" t="str">
-        <v>SPIRITS | WHISKEY</v>
+        <v>WINE | CABERNET SAUVIGNON | RED</v>
       </c>
       <c r="AG10" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH10">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AI10" t="str">
-        <v>visible</v>
+        <v>featured</v>
       </c>
       <c r="AJ10" t="str">
         <v>simple</v>
@@ -1808,7 +1820,7 @@
         <v>open</v>
       </c>
       <c r="AS10" t="str">
-        <v/>
+        <v>RED</v>
       </c>
       <c r="AT10" t="b">
         <v>1</v>
@@ -1816,19 +1828,19 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="str">
-        <v>Caymus Cabernet Sauvignon</v>
+        <v>Kim Crawford Sauvignon Blanc</v>
       </c>
       <c r="D11" t="str">
-        <v>Caymus Cabernet Sauvignon</v>
+        <v>Kim Crawford Sauvignon Blanc</v>
       </c>
       <c r="E11" t="str">
-        <v>A rich, deeply colored and concentrated Cabernet from Napa Valley with scents of dark berries, currants and sweet vanilla oak.</v>
+        <v>An exuberant wine brimming with juicy acidity and fruit sweetness, providing a balanced flavor profile with a lingering finish.</v>
       </c>
       <c r="F11" t="str">
         <v>wine</v>
@@ -1837,52 +1849,52 @@
         <v>WINE</v>
       </c>
       <c r="H11" t="str">
-        <v>red</v>
+        <v>white</v>
       </c>
       <c r="I11" t="str">
-        <v>RED</v>
+        <v>WHITE</v>
       </c>
       <c r="J11" t="str">
-        <v xml:space="preserve">RED  </v>
+        <v xml:space="preserve">WHITE  </v>
       </c>
       <c r="K11" t="str">
-        <v>Cabernet Sauvignon</v>
+        <v>Sauvignon Blanc</v>
       </c>
       <c r="L11" t="str">
-        <v>CABERNET SAUVIGNON</v>
+        <v>SAUVIGNON BLANC</v>
       </c>
       <c r="M11" t="str">
-        <v>Caymus Vineyards</v>
+        <v>Kim Crawford</v>
       </c>
       <c r="N11" t="str">
-        <v>CAYMUS VINEYARDS</v>
+        <v>KIM CRAWFORD</v>
       </c>
       <c r="O11" t="str">
-        <v>United States</v>
+        <v>New Zealand</v>
       </c>
       <c r="P11" t="str">
-        <v>UNITED STATES</v>
+        <v>NEW ZEALAND</v>
       </c>
       <c r="Q11" t="str">
-        <v>Napa Valley</v>
+        <v>Marlborough</v>
       </c>
       <c r="R11">
-        <v>89.95</v>
+        <v>19.95</v>
       </c>
       <c r="S11">
-        <v>71.96</v>
+        <v>15.96</v>
       </c>
       <c r="T11">
-        <v>89.95</v>
+        <v>19.95</v>
       </c>
       <c r="U11" t="str">
-        <v>https://ext.same-assets.com/1701767421/4224202088.png</v>
+        <v>https://ext.same-assets.com/1701767421/3754063653.jpeg</v>
       </c>
       <c r="V11" t="str">
-        <v>https://ext.same-assets.com/1701767421/4224202088.png</v>
+        <v>https://ext.same-assets.com/1701767421/3754063653.jpeg</v>
       </c>
       <c r="W11" t="str">
-        <v>A rich, deeply colored and concentrated Cabernet from Napa Valley with scents of dark berries, currants and sweet vanilla oak.</v>
+        <v>An exuberant wine brimming with juicy acidity and fruit sweetness, providing a balanced flavor profile with a lingering finish.</v>
       </c>
       <c r="X11" t="b">
         <v>0</v>
@@ -1897,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="AB11" t="str">
-        <v>14.6%</v>
+        <v>13%</v>
       </c>
       <c r="AC11" t="str">
         <v>750ml</v>
@@ -1909,13 +1921,13 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF11" t="str">
-        <v>WINE | CABERNET SAUVIGNON | RED</v>
+        <v>WINE | SAUVIGNON BLANC | WHITE</v>
       </c>
       <c r="AG11" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH11">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AI11" t="str">
         <v>featured</v>
@@ -1948,81 +1960,81 @@
         <v>open</v>
       </c>
       <c r="AS11" t="str">
-        <v>RED</v>
+        <v>WHITE</v>
       </c>
       <c r="AT11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" t="str">
-        <v>Kim Crawford Sauvignon Blanc</v>
+        <v>Corona Extra</v>
       </c>
       <c r="D12" t="str">
-        <v>Kim Crawford Sauvignon Blanc</v>
+        <v>Corona Extra</v>
       </c>
       <c r="E12" t="str">
-        <v>An exuberant wine brimming with juicy acidity and fruit sweetness, providing a balanced flavor profile with a lingering finish.</v>
+        <v>A light, crisp and refreshing beer with a hint of fruity-honey aroma. Perfect with a wedge of lime on a hot day.</v>
       </c>
       <c r="F12" t="str">
-        <v>wine</v>
+        <v>beer</v>
       </c>
       <c r="G12" t="str">
-        <v>WINE</v>
+        <v>BEER</v>
       </c>
       <c r="H12" t="str">
-        <v>white</v>
+        <v>imported-beer</v>
       </c>
       <c r="I12" t="str">
-        <v>WHITE</v>
+        <v>IMPORTED-BEER</v>
       </c>
       <c r="J12" t="str">
-        <v xml:space="preserve">WHITE  </v>
+        <v xml:space="preserve">IMPORTED-BEER  </v>
       </c>
       <c r="K12" t="str">
-        <v>Sauvignon Blanc</v>
+        <v/>
       </c>
       <c r="L12" t="str">
-        <v>SAUVIGNON BLANC</v>
+        <v/>
       </c>
       <c r="M12" t="str">
-        <v>Kim Crawford</v>
+        <v>Corona</v>
       </c>
       <c r="N12" t="str">
-        <v>KIM CRAWFORD</v>
+        <v>CORONA</v>
       </c>
       <c r="O12" t="str">
-        <v>New Zealand</v>
+        <v>Mexico</v>
       </c>
       <c r="P12" t="str">
-        <v>NEW ZEALAND</v>
+        <v>MEXICO</v>
       </c>
       <c r="Q12" t="str">
-        <v>Marlborough</v>
+        <v/>
       </c>
       <c r="R12">
-        <v>19.95</v>
+        <v>15.99</v>
       </c>
       <c r="S12">
-        <v>15.96</v>
+        <v>12.79</v>
       </c>
       <c r="T12">
-        <v>19.95</v>
+        <v>15.99</v>
       </c>
       <c r="U12" t="str">
-        <v>https://ext.same-assets.com/1701767421/3754063653.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/2183896642.jpeg</v>
       </c>
       <c r="V12" t="str">
-        <v>https://ext.same-assets.com/1701767421/3754063653.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/2183896642.jpeg</v>
       </c>
       <c r="W12" t="str">
-        <v>An exuberant wine brimming with juicy acidity and fruit sweetness, providing a balanced flavor profile with a lingering finish.</v>
+        <v>A light, crisp and refreshing beer with a hint of fruity-honey aroma. Perfect with a wedge of lime on a hot day.</v>
       </c>
       <c r="X12" t="b">
         <v>0</v>
@@ -2034,31 +2046,31 @@
         <v>0</v>
       </c>
       <c r="AA12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB12" t="str">
-        <v>13%</v>
+        <v>4.5%</v>
       </c>
       <c r="AC12" t="str">
-        <v>750ml</v>
+        <v>6 pack - 330ml</v>
       </c>
       <c r="AD12" t="str">
-        <v>750 ML</v>
+        <v>6 pack - 330 ML</v>
       </c>
       <c r="AE12" t="str">
-        <v>1 x 750 ML</v>
+        <v>1 x 6 pack - 330 ML</v>
       </c>
       <c r="AF12" t="str">
-        <v>WINE | SAUVIGNON BLANC | WHITE</v>
+        <v>BEER | IMPORTED</v>
       </c>
       <c r="AG12" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH12">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AI12" t="str">
-        <v>featured</v>
+        <v>visible</v>
       </c>
       <c r="AJ12" t="str">
         <v>simple</v>
@@ -2088,27 +2100,27 @@
         <v>open</v>
       </c>
       <c r="AS12" t="str">
-        <v>WHITE</v>
+        <v/>
       </c>
       <c r="AT12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" t="str">
-        <v>Corona Extra</v>
+        <v>Heineken Lager</v>
       </c>
       <c r="D13" t="str">
-        <v>Corona Extra</v>
+        <v>Heineken Lager</v>
       </c>
       <c r="E13" t="str">
-        <v>A light, crisp and refreshing beer with a hint of fruity-honey aroma. Perfect with a wedge of lime on a hot day.</v>
+        <v>A clean, crisp and slightly bitter taste. Its refreshing character gives it universal appeal.</v>
       </c>
       <c r="F13" t="str">
         <v>beer</v>
@@ -2132,37 +2144,37 @@
         <v/>
       </c>
       <c r="M13" t="str">
-        <v>Corona</v>
+        <v>Heineken</v>
       </c>
       <c r="N13" t="str">
-        <v>CORONA</v>
+        <v>HEINEKEN</v>
       </c>
       <c r="O13" t="str">
-        <v>Mexico</v>
+        <v>Netherlands</v>
       </c>
       <c r="P13" t="str">
-        <v>MEXICO</v>
+        <v>NETHERLANDS</v>
       </c>
       <c r="Q13" t="str">
         <v/>
       </c>
       <c r="R13">
-        <v>15.99</v>
+        <v>16.99</v>
       </c>
       <c r="S13">
-        <v>12.79</v>
+        <v>13.59</v>
       </c>
       <c r="T13">
-        <v>15.99</v>
+        <v>16.99</v>
       </c>
       <c r="U13" t="str">
-        <v>https://ext.same-assets.com/1701767421/2183896642.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/2445671703.jpeg</v>
       </c>
       <c r="V13" t="str">
-        <v>https://ext.same-assets.com/1701767421/2183896642.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/2445671703.jpeg</v>
       </c>
       <c r="W13" t="str">
-        <v>A light, crisp and refreshing beer with a hint of fruity-honey aroma. Perfect with a wedge of lime on a hot day.</v>
+        <v>A clean, crisp and slightly bitter taste. Its refreshing character gives it universal appeal.</v>
       </c>
       <c r="X13" t="b">
         <v>0</v>
@@ -2177,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="AB13" t="str">
-        <v>4.5%</v>
+        <v>5%</v>
       </c>
       <c r="AC13" t="str">
         <v>6 pack - 330ml</v>
@@ -2195,7 +2207,7 @@
         <v>3 LB</v>
       </c>
       <c r="AH13">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AI13" t="str">
         <v>visible</v>
@@ -2231,24 +2243,24 @@
         <v/>
       </c>
       <c r="AT13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="str">
-        <v>Heineken Lager</v>
+        <v>Budweiser</v>
       </c>
       <c r="D14" t="str">
-        <v>Heineken Lager</v>
+        <v>Budweiser</v>
       </c>
       <c r="E14" t="str">
-        <v>A clean, crisp and slightly bitter taste. Its refreshing character gives it universal appeal.</v>
+        <v>Known as the 'King of Beers,' Budweiser is a medium-bodied, flavorful, crisp American-style lager.</v>
       </c>
       <c r="F14" t="str">
         <v>beer</v>
@@ -2257,13 +2269,13 @@
         <v>BEER</v>
       </c>
       <c r="H14" t="str">
-        <v>imported-beer</v>
+        <v>domestic-beer</v>
       </c>
       <c r="I14" t="str">
-        <v>IMPORTED-BEER</v>
+        <v>DOMESTIC-BEER</v>
       </c>
       <c r="J14" t="str">
-        <v xml:space="preserve">IMPORTED-BEER  </v>
+        <v xml:space="preserve">DOMESTIC-BEER  </v>
       </c>
       <c r="K14" t="str">
         <v/>
@@ -2272,37 +2284,37 @@
         <v/>
       </c>
       <c r="M14" t="str">
-        <v>Heineken</v>
+        <v>Budweiser</v>
       </c>
       <c r="N14" t="str">
-        <v>HEINEKEN</v>
+        <v>BUDWEISER</v>
       </c>
       <c r="O14" t="str">
-        <v>Netherlands</v>
+        <v>United States</v>
       </c>
       <c r="P14" t="str">
-        <v>NETHERLANDS</v>
+        <v>UNITED STATES</v>
       </c>
       <c r="Q14" t="str">
         <v/>
       </c>
       <c r="R14">
-        <v>16.99</v>
+        <v>14.99</v>
       </c>
       <c r="S14">
-        <v>13.59</v>
+        <v>11.99</v>
       </c>
       <c r="T14">
-        <v>16.99</v>
+        <v>14.99</v>
       </c>
       <c r="U14" t="str">
-        <v>https://ext.same-assets.com/1701767421/2445671703.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/999813308.png</v>
       </c>
       <c r="V14" t="str">
-        <v>https://ext.same-assets.com/1701767421/2445671703.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/999813308.png</v>
       </c>
       <c r="W14" t="str">
-        <v>A clean, crisp and slightly bitter taste. Its refreshing character gives it universal appeal.</v>
+        <v>Known as the 'King of Beers,' Budweiser is a medium-bodied, flavorful, crisp American-style lager.</v>
       </c>
       <c r="X14" t="b">
         <v>0</v>
@@ -2320,22 +2332,22 @@
         <v>5%</v>
       </c>
       <c r="AC14" t="str">
-        <v>6 pack - 330ml</v>
+        <v>6 pack - 355ml</v>
       </c>
       <c r="AD14" t="str">
-        <v>6 pack - 330 ML</v>
+        <v>6 pack - 355 ML</v>
       </c>
       <c r="AE14" t="str">
-        <v>1 x 6 pack - 330 ML</v>
+        <v>1 x 6 pack - 355 ML</v>
       </c>
       <c r="AF14" t="str">
-        <v>BEER | IMPORTED</v>
+        <v>BEER | DOMESTIC</v>
       </c>
       <c r="AG14" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH14">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AI14" t="str">
         <v>visible</v>
@@ -2376,19 +2388,19 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="str">
-        <v>Budweiser</v>
+        <v>Stella Artois</v>
       </c>
       <c r="D15" t="str">
-        <v>Budweiser</v>
+        <v>Stella Artois</v>
       </c>
       <c r="E15" t="str">
-        <v>Known as the 'King of Beers,' Budweiser is a medium-bodied, flavorful, crisp American-style lager.</v>
+        <v>A classic Belgian pilsner with a noble hop aroma and a refreshing, crisp taste. Perfect for pairing with food or enjoying on its own.</v>
       </c>
       <c r="F15" t="str">
         <v>beer</v>
@@ -2397,13 +2409,13 @@
         <v>BEER</v>
       </c>
       <c r="H15" t="str">
-        <v>domestic-beer</v>
+        <v>imported-beer</v>
       </c>
       <c r="I15" t="str">
-        <v>DOMESTIC-BEER</v>
+        <v>IMPORTED-BEER</v>
       </c>
       <c r="J15" t="str">
-        <v xml:space="preserve">DOMESTIC-BEER  </v>
+        <v xml:space="preserve">IMPORTED-BEER  </v>
       </c>
       <c r="K15" t="str">
         <v/>
@@ -2412,37 +2424,37 @@
         <v/>
       </c>
       <c r="M15" t="str">
-        <v>Budweiser</v>
+        <v>Stella Artois</v>
       </c>
       <c r="N15" t="str">
-        <v>BUDWEISER</v>
+        <v>STELLA ARTOIS</v>
       </c>
       <c r="O15" t="str">
-        <v>United States</v>
+        <v>Belgium</v>
       </c>
       <c r="P15" t="str">
-        <v>UNITED STATES</v>
+        <v>BELGIUM</v>
       </c>
       <c r="Q15" t="str">
         <v/>
       </c>
       <c r="R15">
-        <v>14.99</v>
+        <v>17.99</v>
       </c>
       <c r="S15">
-        <v>11.99</v>
+        <v>14.39</v>
       </c>
       <c r="T15">
-        <v>14.99</v>
+        <v>17.99</v>
       </c>
       <c r="U15" t="str">
-        <v>https://ext.same-assets.com/1701767421/999813308.png</v>
+        <v>https://ext.same-assets.com/1701767421/3676044092.jpeg</v>
       </c>
       <c r="V15" t="str">
-        <v>https://ext.same-assets.com/1701767421/999813308.png</v>
+        <v>https://ext.same-assets.com/1701767421/3676044092.jpeg</v>
       </c>
       <c r="W15" t="str">
-        <v>Known as the 'King of Beers,' Budweiser is a medium-bodied, flavorful, crisp American-style lager.</v>
+        <v>A classic Belgian pilsner with a noble hop aroma and a refreshing, crisp taste. Perfect for pairing with food or enjoying on its own.</v>
       </c>
       <c r="X15" t="b">
         <v>0</v>
@@ -2457,25 +2469,25 @@
         <v>0</v>
       </c>
       <c r="AB15" t="str">
-        <v>5%</v>
+        <v>5.2%</v>
       </c>
       <c r="AC15" t="str">
-        <v>6 pack - 355ml</v>
+        <v>6 pack - 330ml</v>
       </c>
       <c r="AD15" t="str">
-        <v>6 pack - 355 ML</v>
+        <v>6 pack - 330 ML</v>
       </c>
       <c r="AE15" t="str">
-        <v>1 x 6 pack - 355 ML</v>
+        <v>1 x 6 pack - 330 ML</v>
       </c>
       <c r="AF15" t="str">
-        <v>BEER | DOMESTIC</v>
+        <v>BEER | IMPORTED</v>
       </c>
       <c r="AG15" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH15">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AI15" t="str">
         <v>visible</v>
@@ -2516,34 +2528,34 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" t="str">
-        <v>Stella Artois</v>
+        <v>Casamigos Blanco Tequila</v>
       </c>
       <c r="D16" t="str">
-        <v>Stella Artois</v>
+        <v>Casamigos Blanco Tequila</v>
       </c>
       <c r="E16" t="str">
-        <v>A classic Belgian pilsner with a noble hop aroma and a refreshing, crisp taste. Perfect for pairing with food or enjoying on its own.</v>
+        <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
       </c>
       <c r="F16" t="str">
-        <v>beer</v>
+        <v>spirits</v>
       </c>
       <c r="G16" t="str">
-        <v>BEER</v>
+        <v>SPIRITS</v>
       </c>
       <c r="H16" t="str">
-        <v>imported-beer</v>
+        <v>tequila</v>
       </c>
       <c r="I16" t="str">
-        <v>IMPORTED-BEER</v>
+        <v>TEQUILA</v>
       </c>
       <c r="J16" t="str">
-        <v xml:space="preserve">IMPORTED-BEER  </v>
+        <v xml:space="preserve">TEQUILA  </v>
       </c>
       <c r="K16" t="str">
         <v/>
@@ -2552,40 +2564,40 @@
         <v/>
       </c>
       <c r="M16" t="str">
-        <v>Stella Artois</v>
+        <v>Casamigos</v>
       </c>
       <c r="N16" t="str">
-        <v>STELLA ARTOIS</v>
+        <v>CASAMIGOS</v>
       </c>
       <c r="O16" t="str">
-        <v>Belgium</v>
+        <v>Mexico</v>
       </c>
       <c r="P16" t="str">
-        <v>BELGIUM</v>
+        <v>MEXICO</v>
       </c>
       <c r="Q16" t="str">
-        <v/>
+        <v>Jalisco</v>
       </c>
       <c r="R16">
-        <v>17.99</v>
+        <v>49.99</v>
       </c>
       <c r="S16">
-        <v>14.39</v>
+        <v>39.99</v>
       </c>
       <c r="T16">
-        <v>17.99</v>
+        <v>49.99</v>
       </c>
       <c r="U16" t="str">
-        <v>https://ext.same-assets.com/1701767421/3676044092.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/1355704146.jpeg</v>
       </c>
       <c r="V16" t="str">
-        <v>https://ext.same-assets.com/1701767421/3676044092.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/1355704146.jpeg</v>
       </c>
       <c r="W16" t="str">
-        <v>A classic Belgian pilsner with a noble hop aroma and a refreshing, crisp taste. Perfect for pairing with food or enjoying on its own.</v>
+        <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
       </c>
       <c r="X16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" t="b">
         <v>0</v>
@@ -2594,31 +2606,31 @@
         <v>0</v>
       </c>
       <c r="AA16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB16" t="str">
-        <v>5.2%</v>
+        <v>40%</v>
       </c>
       <c r="AC16" t="str">
-        <v>6 pack - 330ml</v>
+        <v>750ml</v>
       </c>
       <c r="AD16" t="str">
-        <v>6 pack - 330 ML</v>
+        <v>750 ML</v>
       </c>
       <c r="AE16" t="str">
-        <v>1 x 6 pack - 330 ML</v>
+        <v>1 x 750 ML</v>
       </c>
       <c r="AF16" t="str">
-        <v>BEER | IMPORTED</v>
+        <v>SPIRITS | TEQUILA</v>
       </c>
       <c r="AG16" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI16" t="str">
-        <v>visible</v>
+        <v>featured</v>
       </c>
       <c r="AJ16" t="str">
         <v>simple</v>
@@ -2651,81 +2663,81 @@
         <v/>
       </c>
       <c r="AT16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" t="str">
-        <v>Casamigos Blanco Tequila</v>
+        <v>Moët &amp; Chandon Impérial Brut</v>
       </c>
       <c r="D17" t="str">
-        <v>Casamigos Blanco Tequila</v>
+        <v>Moët &amp; Chandon Impérial Brut</v>
       </c>
       <c r="E17" t="str">
-        <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
+        <v>A harmonious blend of the three wine varieties, offering bright fruitiness, a seductive palate and an elegant maturity.</v>
       </c>
       <c r="F17" t="str">
-        <v>spirits</v>
+        <v>wine</v>
       </c>
       <c r="G17" t="str">
-        <v>SPIRITS</v>
+        <v>WINE</v>
       </c>
       <c r="H17" t="str">
-        <v>tequila</v>
+        <v>champagne</v>
       </c>
       <c r="I17" t="str">
-        <v>TEQUILA</v>
+        <v>CHAMPAGNE</v>
       </c>
       <c r="J17" t="str">
-        <v xml:space="preserve">TEQUILA  </v>
+        <v xml:space="preserve">CHAMPAGNE  </v>
       </c>
       <c r="K17" t="str">
-        <v/>
+        <v>Champagne Blend</v>
       </c>
       <c r="L17" t="str">
-        <v/>
+        <v>CHAMPAGNE BLEND</v>
       </c>
       <c r="M17" t="str">
-        <v>Casamigos</v>
+        <v>Moët &amp; Chandon</v>
       </c>
       <c r="N17" t="str">
-        <v>CASAMIGOS</v>
+        <v>MOËT &amp; CHANDON</v>
       </c>
       <c r="O17" t="str">
-        <v>Mexico</v>
+        <v>France</v>
       </c>
       <c r="P17" t="str">
-        <v>MEXICO</v>
+        <v>FRANCE</v>
       </c>
       <c r="Q17" t="str">
-        <v>Jalisco</v>
+        <v>Champagne</v>
       </c>
       <c r="R17">
-        <v>49.99</v>
+        <v>59.95</v>
       </c>
       <c r="S17">
-        <v>39.99</v>
+        <v>47.96</v>
       </c>
       <c r="T17">
-        <v>49.99</v>
+        <v>59.95</v>
       </c>
       <c r="U17" t="str">
-        <v>https://ext.same-assets.com/1701767421/1355704146.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/1204111697.jpeg</v>
       </c>
       <c r="V17" t="str">
-        <v>https://ext.same-assets.com/1701767421/1355704146.jpeg</v>
+        <v>https://ext.same-assets.com/1701767421/1204111697.jpeg</v>
       </c>
       <c r="W17" t="str">
-        <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
+        <v>A harmonious blend of the three wine varieties, offering bright fruitiness, a seductive palate and an elegant maturity.</v>
       </c>
       <c r="X17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" t="b">
         <v>0</v>
@@ -2737,7 +2749,7 @@
         <v>1</v>
       </c>
       <c r="AB17" t="str">
-        <v>40%</v>
+        <v>12%</v>
       </c>
       <c r="AC17" t="str">
         <v>750ml</v>
@@ -2749,13 +2761,13 @@
         <v>1 x 750 ML</v>
       </c>
       <c r="AF17" t="str">
-        <v>SPIRITS | TEQUILA</v>
+        <v>WINE | CHAMPAGNE</v>
       </c>
       <c r="AG17" t="str">
         <v>3 LB</v>
       </c>
       <c r="AH17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AI17" t="str">
         <v>featured</v>
@@ -2788,123 +2800,73 @@
         <v>open</v>
       </c>
       <c r="AS17" t="str">
-        <v/>
+        <v>WHITE</v>
       </c>
       <c r="AT17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>16</v>
+    <row r="18" xml:space="preserve">
+      <c r="A18" t="str">
+        <v>600</v>
+      </c>
+      <c r="B18" t="str">
+        <v>SKU-600-819</v>
       </c>
       <c r="C18" t="str">
-        <v>Moët &amp; Chandon Impérial Brut</v>
+        <v>Late-Night Jazz</v>
       </c>
       <c r="D18" t="str">
-        <v>Moët &amp; Chandon Impérial Brut</v>
+        <v>Late-Night Jazz</v>
       </c>
       <c r="E18" t="str">
-        <v>A harmonious blend of the three wine varieties, offering bright fruitiness, a seductive palate and an elegant maturity.</v>
+        <v>Short Description</v>
       </c>
       <c r="F18" t="str">
-        <v>wine</v>
+        <v>spirits</v>
       </c>
       <c r="G18" t="str">
-        <v>WINE</v>
+        <v>spirits</v>
       </c>
       <c r="H18" t="str">
-        <v>champagne</v>
-      </c>
-      <c r="I18" t="str">
-        <v>CHAMPAGNE</v>
-      </c>
-      <c r="J18" t="str">
-        <v xml:space="preserve">CHAMPAGNE  </v>
-      </c>
-      <c r="K18" t="str">
-        <v>Champagne Blend</v>
-      </c>
-      <c r="L18" t="str">
-        <v>CHAMPAGNE BLEND</v>
+        <v>domestic-beer</v>
       </c>
       <c r="M18" t="str">
-        <v>Moët &amp; Chandon</v>
+        <v>Don Julio</v>
       </c>
       <c r="N18" t="str">
-        <v>MOËT &amp; CHANDON</v>
+        <v>Don Julio</v>
       </c>
       <c r="O18" t="str">
-        <v>France</v>
-      </c>
-      <c r="P18" t="str">
-        <v>FRANCE</v>
-      </c>
-      <c r="Q18" t="str">
-        <v>Champagne</v>
+        <v>Scotland</v>
       </c>
       <c r="R18">
-        <v>59.95</v>
-      </c>
-      <c r="S18">
-        <v>47.96</v>
+        <v>12</v>
       </c>
       <c r="T18">
-        <v>59.95</v>
+        <v>12</v>
       </c>
       <c r="U18" t="str">
-        <v>https://ext.same-assets.com/1701767421/1204111697.jpeg</v>
-      </c>
-      <c r="V18" t="str">
-        <v>https://ext.same-assets.com/1701767421/1204111697.jpeg</v>
-      </c>
-      <c r="W18" t="str">
-        <v>A harmonious blend of the three wine varieties, offering bright fruitiness, a seductive palate and an elegant maturity.</v>
-      </c>
-      <c r="X18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB18" t="str">
-        <v>12%</v>
-      </c>
-      <c r="AC18" t="str">
-        <v>750ml</v>
-      </c>
-      <c r="AD18" t="str">
-        <v>750 ML</v>
-      </c>
-      <c r="AE18" t="str">
-        <v>1 x 750 ML</v>
-      </c>
-      <c r="AF18" t="str">
-        <v>WINE | CHAMPAGNE</v>
-      </c>
-      <c r="AG18" t="str">
-        <v>3 LB</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164255/ecflqfgmdsjytlyjsgvo.jpg</v>
+      </c>
+      <c r="W18" t="str" xml:space="preserve">
+        <v xml:space="preserve">Description
+</v>
+      </c>
+      <c r="X18" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y18" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z18" t="str">
+        <v>false</v>
+      </c>
+      <c r="AA18" t="str">
+        <v>false</v>
       </c>
       <c r="AH18">
-        <v>10</v>
-      </c>
-      <c r="AI18" t="str">
-        <v>featured</v>
-      </c>
-      <c r="AJ18" t="str">
-        <v>simple</v>
-      </c>
-      <c r="AK18" t="str">
-        <v>yes</v>
+        <v>11</v>
       </c>
       <c r="AL18" t="str">
         <v>taxable</v>
@@ -2918,71 +2880,82 @@
       <c r="AO18" t="str">
         <v>instock</v>
       </c>
-      <c r="AP18" t="str">
-        <v>visible</v>
-      </c>
       <c r="AQ18" t="str">
         <v>publish</v>
       </c>
       <c r="AR18" t="str">
         <v>open</v>
       </c>
-      <c r="AS18" t="str">
-        <v>WHITE</v>
-      </c>
-      <c r="AT18" t="b">
-        <v>1</v>
+      <c r="AT18" t="str">
+        <v>false</v>
+      </c>
+      <c r="AU18" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164255/ecflqfgmdsjytlyjsgvo.jpg</v>
+      </c>
+      <c r="AV18" t="str">
+        <v>2025-03-28T12:17:35.575Z</v>
+      </c>
+      <c r="AW18" t="str">
+        <v>600</v>
+      </c>
+      <c r="AX18" t="str">
+        <v>2025-03-28T12:17:35.575Z</v>
       </c>
     </row>
-    <row r="19" xml:space="preserve">
+    <row r="19">
       <c r="A19" t="str">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B19" t="str">
-        <v>SKU-600-819</v>
+        <v>SKU-601-929</v>
       </c>
       <c r="C19" t="str">
-        <v>Late-Night Jazz</v>
+        <v>Sameer</v>
       </c>
       <c r="D19" t="str">
-        <v>Late-Night Jazz</v>
+        <v>Sameer</v>
       </c>
       <c r="E19" t="str">
-        <v>Short Description</v>
+        <v>Short Description test</v>
       </c>
       <c r="F19" t="str">
-        <v>spirits</v>
+        <v>wine</v>
       </c>
       <c r="G19" t="str">
-        <v>spirits</v>
+        <v>wine</v>
       </c>
       <c r="H19" t="str">
-        <v>domestic-beer</v>
+        <v>whiskey</v>
       </c>
       <c r="M19" t="str">
-        <v>Don Julio</v>
+        <v>Heineken</v>
       </c>
       <c r="N19" t="str">
-        <v>Don Julio</v>
+        <v>Heineken</v>
       </c>
       <c r="O19" t="str">
-        <v>Scotland</v>
+        <v>Belgium</v>
+      </c>
+      <c r="Q19" t="str">
+        <v>Asia</v>
       </c>
       <c r="R19">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="S19">
+        <v>13</v>
       </c>
       <c r="T19">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="U19" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164255/ecflqfgmdsjytlyjsgvo.jpg</v>
-      </c>
-      <c r="W19" t="str" xml:space="preserve">
-        <v xml:space="preserve">Description
-</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164700/mpdivfgdvuxwibmnh8qj.png</v>
+      </c>
+      <c r="W19" t="str">
+        <v>Description test</v>
       </c>
       <c r="X19" t="str">
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="Y19" t="str">
         <v>false</v>
@@ -2994,13 +2967,13 @@
         <v>false</v>
       </c>
       <c r="AH19">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="AL19" t="str">
         <v>taxable</v>
       </c>
       <c r="AM19" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="AN19" t="str">
         <v>no</v>
@@ -3018,90 +2991,87 @@
         <v>false</v>
       </c>
       <c r="AU19" t="str">
-        <v>600</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164700/mpdivfgdvuxwibmnh8qj.png</v>
       </c>
       <c r="AV19" t="str">
-        <v>2025-03-28T12:17:35.575Z</v>
+        <v>2025-03-28T12:25:00.293Z</v>
       </c>
       <c r="AW19" t="str">
-        <v>2025-03-28T12:17:35.575Z</v>
+        <v>601</v>
       </c>
       <c r="AX19" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164255/ecflqfgmdsjytlyjsgvo.jpg</v>
+        <v>2025-03-28T12:25:00.293Z</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B20" t="str">
-        <v>SKU-601-929</v>
+        <v>SKU-602-514</v>
       </c>
       <c r="C20" t="str">
-        <v>Sameer</v>
+        <v>Late-Night Jazz2</v>
       </c>
       <c r="D20" t="str">
-        <v>Sameer</v>
+        <v>Late-Night Jazz2</v>
       </c>
       <c r="E20" t="str">
-        <v>Short Description test</v>
+        <v>Short Description</v>
       </c>
       <c r="F20" t="str">
-        <v>wine</v>
+        <v>beer</v>
       </c>
       <c r="G20" t="str">
-        <v>wine</v>
+        <v>beer</v>
       </c>
       <c r="H20" t="str">
-        <v>whiskey</v>
+        <v>gin</v>
       </c>
       <c r="M20" t="str">
-        <v>Heineken</v>
+        <v>Don Julio</v>
       </c>
       <c r="N20" t="str">
-        <v>Heineken</v>
+        <v>Don Julio</v>
       </c>
       <c r="O20" t="str">
-        <v>Belgium</v>
-      </c>
-      <c r="Q20" t="str">
-        <v>Asia</v>
+        <v>Netherlands</v>
       </c>
       <c r="R20">
-        <v>56</v>
-      </c>
-      <c r="S20">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="T20">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="U20" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164700/mpdivfgdvuxwibmnh8qj.png</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165101/dchmyizipoy2zvzbw3pk.png</v>
       </c>
       <c r="W20" t="str">
-        <v>Description test</v>
+        <v>Description</v>
       </c>
       <c r="X20" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y20" t="str">
         <v>true</v>
       </c>
-      <c r="Y20" t="str">
-        <v>false</v>
-      </c>
       <c r="Z20" t="str">
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="AA20" t="str">
-        <v>false</v>
+        <v>true</v>
+      </c>
+      <c r="AC20" t="str">
+        <v>45</v>
       </c>
       <c r="AH20">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="AL20" t="str">
         <v>taxable</v>
       </c>
       <c r="AM20" t="str">
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="AN20" t="str">
         <v>no</v>
@@ -3116,81 +3086,81 @@
         <v>open</v>
       </c>
       <c r="AT20" t="str">
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="AU20" t="str">
-        <v>601</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165101/dchmyizipoy2zvzbw3pk.png</v>
       </c>
       <c r="AV20" t="str">
-        <v>2025-03-28T12:25:00.293Z</v>
+        <v>2025-03-28T12:31:41.045Z</v>
       </c>
       <c r="AW20" t="str">
-        <v>2025-03-28T12:25:00.293Z</v>
+        <v>602</v>
       </c>
       <c r="AX20" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743164700/mpdivfgdvuxwibmnh8qj.png</v>
+        <v>2025-03-28T12:31:41.045Z</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B21" t="str">
-        <v>SKU-602-514</v>
+        <v>SKU-603-477</v>
       </c>
       <c r="C21" t="str">
-        <v>Late-Night Jazz2</v>
+        <v>sd</v>
       </c>
       <c r="D21" t="str">
-        <v>Late-Night Jazz2</v>
+        <v>sd</v>
       </c>
       <c r="E21" t="str">
         <v>Short Description</v>
       </c>
       <c r="F21" t="str">
-        <v>beer</v>
+        <v>wine</v>
       </c>
       <c r="G21" t="str">
-        <v>beer</v>
+        <v>wine</v>
       </c>
       <c r="H21" t="str">
         <v>gin</v>
       </c>
       <c r="M21" t="str">
-        <v>Don Julio</v>
+        <v>Jack Daniel's</v>
       </c>
       <c r="N21" t="str">
-        <v>Don Julio</v>
+        <v>Jack Daniel's</v>
       </c>
       <c r="O21" t="str">
-        <v>Netherlands</v>
+        <v>France</v>
       </c>
       <c r="R21">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="T21">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="U21" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165101/dchmyizipoy2zvzbw3pk.png</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165990/ink5annljlba5t43evp9.png</v>
       </c>
       <c r="W21" t="str">
         <v>Description</v>
       </c>
       <c r="X21" t="str">
+        <v>true</v>
+      </c>
+      <c r="Y21" t="str">
         <v>false</v>
       </c>
-      <c r="Y21" t="str">
-        <v>true</v>
-      </c>
       <c r="Z21" t="str">
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="AA21" t="str">
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="AC21" t="str">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="AH21">
         <v>12</v>
@@ -3214,33 +3184,33 @@
         <v>open</v>
       </c>
       <c r="AT21" t="str">
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="AU21" t="str">
-        <v>602</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165990/ink5annljlba5t43evp9.png</v>
       </c>
       <c r="AV21" t="str">
-        <v>2025-03-28T12:31:41.045Z</v>
+        <v>2025-03-28T12:46:29.945Z</v>
       </c>
       <c r="AW21" t="str">
-        <v>2025-03-28T12:31:41.045Z</v>
+        <v>603</v>
       </c>
       <c r="AX21" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165101/dchmyizipoy2zvzbw3pk.png</v>
+        <v>2025-03-28T12:46:29.945Z</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B22" t="str">
-        <v>SKU-603-477</v>
+        <v>SKU-604-255</v>
       </c>
       <c r="C22" t="str">
-        <v>sd</v>
+        <v>waefds</v>
       </c>
       <c r="D22" t="str">
-        <v>sd</v>
+        <v>waefds</v>
       </c>
       <c r="E22" t="str">
         <v>Short Description</v>
@@ -3252,46 +3222,49 @@
         <v>wine</v>
       </c>
       <c r="H22" t="str">
-        <v>gin</v>
+        <v>vodka</v>
+      </c>
+      <c r="K22" t="str">
+        <v>Sauvignon Blanc</v>
       </c>
       <c r="M22" t="str">
-        <v>Jack Daniel's</v>
+        <v>Corona</v>
       </c>
       <c r="N22" t="str">
-        <v>Jack Daniel's</v>
+        <v>Corona</v>
       </c>
       <c r="O22" t="str">
-        <v>France</v>
+        <v>United States</v>
       </c>
       <c r="R22">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="T22">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="U22" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165990/ink5annljlba5t43evp9.png</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743167761/ze72ozlwshblwqgedtus.webp</v>
       </c>
       <c r="W22" t="str">
-        <v>Description</v>
+        <v>Description 69 stock products</v>
       </c>
       <c r="X22" t="str">
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="Y22" t="str">
         <v>false</v>
       </c>
       <c r="Z22" t="str">
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="AA22" t="str">
         <v>false</v>
       </c>
       <c r="AC22" t="str">
-        <v>89</v>
+        <v>567</v>
       </c>
       <c r="AH22">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="AL22" t="str">
         <v>taxable</v>
@@ -3315,30 +3288,30 @@
         <v>false</v>
       </c>
       <c r="AU22" t="str">
-        <v>603</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743167761/ze72ozlwshblwqgedtus.webp</v>
       </c>
       <c r="AV22" t="str">
-        <v>2025-03-28T12:46:29.945Z</v>
+        <v>2025-03-28T13:16:01.109Z</v>
       </c>
       <c r="AW22" t="str">
-        <v>2025-03-28T12:46:29.945Z</v>
+        <v>604</v>
       </c>
       <c r="AX22" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743165990/ink5annljlba5t43evp9.png</v>
+        <v>2025-03-28T13:16:01.109Z</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B23" t="str">
-        <v>SKU-604-255</v>
+        <v>SKU-605-622</v>
       </c>
       <c r="C23" t="str">
-        <v>waefds</v>
+        <v>wrapper2</v>
       </c>
       <c r="D23" t="str">
-        <v>waefds</v>
+        <v>wrapper2</v>
       </c>
       <c r="E23" t="str">
         <v>Short Description</v>
@@ -3349,32 +3322,23 @@
       <c r="G23" t="str">
         <v>wine</v>
       </c>
-      <c r="H23" t="str">
-        <v>vodka</v>
-      </c>
-      <c r="K23" t="str">
-        <v>Sauvignon Blanc</v>
-      </c>
       <c r="M23" t="str">
-        <v>Corona</v>
+        <v>Jack Daniel's</v>
       </c>
       <c r="N23" t="str">
-        <v>Corona</v>
-      </c>
-      <c r="O23" t="str">
-        <v>United States</v>
+        <v>Jack Daniel's</v>
       </c>
       <c r="R23">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="T23">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="U23" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743167761/ze72ozlwshblwqgedtus.webp</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743173157/uuda9jladhmshjeszkr1.jpg</v>
       </c>
       <c r="W23" t="str">
-        <v>Description 69 stock products</v>
+        <v>Short Description</v>
       </c>
       <c r="X23" t="str">
         <v>false</v>
@@ -3389,10 +3353,13 @@
         <v>false</v>
       </c>
       <c r="AC23" t="str">
-        <v>567</v>
+        <v>12</v>
+      </c>
+      <c r="AD23" t="str">
+        <v>12</v>
       </c>
       <c r="AH23">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="AL23" t="str">
         <v>taxable</v>
@@ -3416,21 +3383,107 @@
         <v>false</v>
       </c>
       <c r="AU23" t="str">
-        <v>604</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743173157/uuda9jladhmshjeszkr1.jpg</v>
       </c>
       <c r="AV23" t="str">
-        <v>2025-03-28T13:16:01.109Z</v>
+        <v>2025-03-28T15:06:54.834Z</v>
       </c>
       <c r="AW23" t="str">
-        <v>2025-03-28T13:16:01.109Z</v>
+        <v>605</v>
       </c>
       <c r="AX23" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743167761/ze72ozlwshblwqgedtus.webp</v>
+        <v>2025-03-28T14:45:57.115Z</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>606</v>
+      </c>
+      <c r="B24" t="str">
+        <v>SKU-606-998</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Late-Night Jazz</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Late-Night Jazz</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Descriptions</v>
+      </c>
+      <c r="F24" t="str">
+        <v>spirits</v>
+      </c>
+      <c r="G24" t="str">
+        <v>spirits</v>
+      </c>
+      <c r="R24">
+        <v>34</v>
+      </c>
+      <c r="T24">
+        <v>34</v>
+      </c>
+      <c r="U24" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743174957/gkmedfirj67byqafpo36.png</v>
+      </c>
+      <c r="W24" t="str">
+        <v>Descriptions</v>
+      </c>
+      <c r="X24" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y24" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z24" t="str">
+        <v>true</v>
+      </c>
+      <c r="AA24" t="str">
+        <v>false</v>
+      </c>
+      <c r="AC24" t="str">
+        <v>34</v>
+      </c>
+      <c r="AH24">
+        <v>34</v>
+      </c>
+      <c r="AL24" t="str">
+        <v>taxable</v>
+      </c>
+      <c r="AM24" t="str">
+        <v>no</v>
+      </c>
+      <c r="AN24" t="str">
+        <v>no</v>
+      </c>
+      <c r="AO24" t="str">
+        <v>instock</v>
+      </c>
+      <c r="AQ24" t="str">
+        <v>publish</v>
+      </c>
+      <c r="AR24" t="str">
+        <v>open</v>
+      </c>
+      <c r="AT24" t="str">
+        <v>false</v>
+      </c>
+      <c r="AU24" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743174957/gkmedfirj67byqafpo36.png</v>
+      </c>
+      <c r="AV24" t="str">
+        <v>2025-03-28T15:15:57.426Z</v>
+      </c>
+      <c r="AW24" t="str">
+        <v>606</v>
+      </c>
+      <c r="AX24" t="str">
+        <v>2025-03-28T15:15:57.426Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AX23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AX24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Categories, brands, types and varietals apis made
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -644,7 +644,7 @@
         <v>750ml</v>
       </c>
       <c r="AC2" t="str">
-        <v>750ML</v>
+        <v>750 ML</v>
       </c>
       <c r="AD2" t="str">
         <v>1 x 750 ML</v>
@@ -698,10 +698,7 @@
         <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="AU2" t="str">
-        <v>2025-03-29T03:58:24.808Z</v>
-      </c>
-      <c r="AV2" t="str">
-        <v>wine</v>
+        <v>2025-03-29T02:10:07.293Z</v>
       </c>
     </row>
     <row r="3">
@@ -998,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="str">
-        <v>Grey Goose Vodka</v>
+        <v>Grey Goose Vodka 34</v>
       </c>
       <c r="D5" t="str">
         <v>Grey Goose Vodka</v>
@@ -3449,13 +3446,10 @@
         <v>false</v>
       </c>
       <c r="AB24" t="str">
+        <v>34ml</v>
+      </c>
+      <c r="AG24">
         <v>34</v>
-      </c>
-      <c r="AC24" t="str">
-        <v>34ML</v>
-      </c>
-      <c r="AG24">
-        <v>33.98</v>
       </c>
       <c r="AK24" t="str">
         <v>taxable</v>
@@ -3482,7 +3476,7 @@
         <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743174957/gkmedfirj67byqafpo36.png</v>
       </c>
       <c r="AU24" t="str">
-        <v>2025-03-29T03:41:57.723Z</v>
+        <v>2025-03-28T15:15:57.426Z</v>
       </c>
       <c r="AV24" t="str">
         <v>spirits</v>
@@ -3495,110 +3489,74 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="str">
+      <c r="A25">
         <v>607</v>
       </c>
       <c r="B25" t="str">
-        <v>SKU-607-670</v>
+        <v>SKU-606-999</v>
       </c>
       <c r="C25" t="str">
-        <v>Three tier architecture</v>
+        <v>test</v>
       </c>
       <c r="D25" t="str">
-        <v>Three tier architecture</v>
+        <v>test</v>
       </c>
       <c r="E25" t="str">
-        <v>Short Description</v>
+        <v>test</v>
       </c>
       <c r="F25" t="str">
-        <v>wine</v>
+        <v>test category 34</v>
       </c>
       <c r="G25" t="str">
-        <v>whiskey</v>
+        <v>test</v>
+      </c>
+      <c r="H25" t="str">
+        <v>test</v>
+      </c>
+      <c r="I25" t="str">
+        <v>test</v>
+      </c>
+      <c r="J25" t="str">
+        <v>test</v>
+      </c>
+      <c r="K25" t="str">
+        <v>test</v>
       </c>
       <c r="L25" t="str">
-        <v>Grey Goose</v>
+        <v>test</v>
       </c>
       <c r="M25" t="str">
-        <v>Grey Goose</v>
+        <v>test</v>
       </c>
       <c r="N25" t="str">
-        <v>Scotland</v>
+        <v>test</v>
       </c>
       <c r="O25" t="str">
-        <v>Scotland</v>
+        <v>test</v>
+      </c>
+      <c r="P25" t="str">
+        <v>test</v>
       </c>
       <c r="Q25">
-        <v>23</v>
+        <v>56</v>
+      </c>
+      <c r="R25">
+        <v>56</v>
       </c>
       <c r="S25">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="T25" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743220224/cwylnxb4ojuap4mwpko8.png</v>
-      </c>
-      <c r="V25" t="str">
-        <v>Description</v>
-      </c>
-      <c r="W25" t="str">
-        <v>false</v>
-      </c>
-      <c r="X25" t="str">
-        <v>false</v>
-      </c>
-      <c r="Y25" t="str">
-        <v>true</v>
-      </c>
-      <c r="Z25" t="str">
-        <v>true</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743174957/gkmedfirj67byqafpo36.png</v>
       </c>
       <c r="AB25" t="str">
-        <v>69ml</v>
-      </c>
-      <c r="AC25" t="str">
-        <v>69ML</v>
+        <v>76ml</v>
       </c>
       <c r="AG25">
-        <v>23</v>
-      </c>
-      <c r="AI25" t="str">
-        <v>whiskey</v>
-      </c>
-      <c r="AK25" t="str">
-        <v>taxable</v>
-      </c>
-      <c r="AL25" t="str">
-        <v>no</v>
-      </c>
-      <c r="AM25" t="str">
-        <v>no</v>
-      </c>
-      <c r="AN25" t="str">
-        <v>instock</v>
-      </c>
-      <c r="AP25" t="str">
-        <v>publish</v>
-      </c>
-      <c r="AQ25" t="str">
-        <v>open</v>
-      </c>
-      <c r="AS25" t="str">
-        <v>false</v>
-      </c>
-      <c r="AT25" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743220224/cwylnxb4ojuap4mwpko8.png</v>
-      </c>
-      <c r="AU25" t="str">
-        <v>2025-03-29T03:58:45.808Z</v>
+        <v>76</v>
       </c>
       <c r="AV25" t="str">
-        <v>wine</v>
-      </c>
-      <c r="AW25" t="str">
-        <v>607</v>
-      </c>
-      <c r="AX25" t="str">
-        <v>2025-03-29T03:50:25.423Z</v>
+        <v>test category</v>
       </c>
     </row>
     <row r="26">
@@ -3606,16 +3564,19 @@
         <v>608</v>
       </c>
       <c r="B26" t="str">
-        <v>SKU-608-351</v>
+        <v>SKU-608-717</v>
       </c>
       <c r="C26" t="str">
-        <v>Five Stage Pipeline</v>
+        <v>test product</v>
       </c>
       <c r="D26" t="str">
-        <v>Five Stage Pipeline</v>
+        <v>test product</v>
       </c>
       <c r="F26" t="str">
-        <v>spirits</v>
+        <v>beer</v>
+      </c>
+      <c r="G26" t="str">
+        <v>whiskey</v>
       </c>
       <c r="Q26">
         <v>34</v>
@@ -3624,7 +3585,7 @@
         <v>34</v>
       </c>
       <c r="T26" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743220798/pdhlwzh1dtyqvxrvmdkq.png</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743226484/vzcjhlpqnvz4i0x2uw1j.svg</v>
       </c>
       <c r="W26" t="str">
         <v>false</v>
@@ -3645,7 +3606,7 @@
         <v>45ML</v>
       </c>
       <c r="AG26">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="AK26" t="str">
         <v>taxable</v>
@@ -3669,19 +3630,19 @@
         <v>false</v>
       </c>
       <c r="AT26" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743220798/pdhlwzh1dtyqvxrvmdkq.png</v>
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743226484/vzcjhlpqnvz4i0x2uw1j.svg</v>
       </c>
       <c r="AU26" t="str">
-        <v>2025-03-29T03:59:59.242Z</v>
+        <v>2025-03-29T05:34:46.251Z</v>
       </c>
       <c r="AV26" t="str">
-        <v>spirits</v>
+        <v>beer</v>
       </c>
       <c r="AW26" t="str">
         <v>608</v>
       </c>
       <c r="AX26" t="str">
-        <v>2025-03-29T03:59:59.242Z</v>
+        <v>2025-03-29T05:34:46.251Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Taxanomy Created and tested
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX26"/>
+  <dimension ref="A1:AX27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -599,7 +599,7 @@
         <v>DOM PÉRIGNON</v>
       </c>
       <c r="N2" t="str">
-        <v>France</v>
+        <v>test2</v>
       </c>
       <c r="O2" t="str">
         <v>FRANCE</v>
@@ -644,7 +644,7 @@
         <v>750ml</v>
       </c>
       <c r="AC2" t="str">
-        <v>750 ML</v>
+        <v>750ML</v>
       </c>
       <c r="AD2" t="str">
         <v>1 x 750 ML</v>
@@ -698,7 +698,10 @@
         <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="AU2" t="str">
-        <v>2025-03-29T02:10:07.293Z</v>
+        <v>2025-03-29T06:55:47.797Z</v>
+      </c>
+      <c r="AV2" t="str">
+        <v>wine</v>
       </c>
     </row>
     <row r="3">
@@ -3645,9 +3648,119 @@
         <v>2025-03-29T05:34:46.251Z</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>609</v>
+      </c>
+      <c r="B27" t="str">
+        <v>SKU-609-858</v>
+      </c>
+      <c r="C27" t="str">
+        <v>category, brand  , country and varietal</v>
+      </c>
+      <c r="D27" t="str">
+        <v>category, brand  , country and varietal</v>
+      </c>
+      <c r="E27" t="str">
+        <v>category, brand  , country and varietal</v>
+      </c>
+      <c r="F27" t="str">
+        <v>TEst</v>
+      </c>
+      <c r="G27" t="str">
+        <v>test2</v>
+      </c>
+      <c r="H27" t="str">
+        <v>test2</v>
+      </c>
+      <c r="J27" t="str">
+        <v>test2</v>
+      </c>
+      <c r="L27" t="str">
+        <v>test2</v>
+      </c>
+      <c r="M27" t="str">
+        <v>test2</v>
+      </c>
+      <c r="N27" t="str">
+        <v>test2</v>
+      </c>
+      <c r="Q27">
+        <v>123</v>
+      </c>
+      <c r="S27">
+        <v>123</v>
+      </c>
+      <c r="T27" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743231607/kds3tizmge75ujw5kqln.png</v>
+      </c>
+      <c r="V27" t="str">
+        <v>category, brand  , country and varietal</v>
+      </c>
+      <c r="W27" t="str">
+        <v>false</v>
+      </c>
+      <c r="X27" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y27" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z27" t="str">
+        <v>false</v>
+      </c>
+      <c r="AB27" t="str">
+        <v>45ml</v>
+      </c>
+      <c r="AC27" t="str">
+        <v>45ML</v>
+      </c>
+      <c r="AG27">
+        <v>123</v>
+      </c>
+      <c r="AI27" t="str">
+        <v>test2</v>
+      </c>
+      <c r="AK27" t="str">
+        <v>taxable</v>
+      </c>
+      <c r="AL27" t="str">
+        <v>no</v>
+      </c>
+      <c r="AM27" t="str">
+        <v>no</v>
+      </c>
+      <c r="AN27" t="str">
+        <v>instock</v>
+      </c>
+      <c r="AP27" t="str">
+        <v>publish</v>
+      </c>
+      <c r="AQ27" t="str">
+        <v>open</v>
+      </c>
+      <c r="AS27" t="str">
+        <v>false</v>
+      </c>
+      <c r="AT27" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743231607/kds3tizmge75ujw5kqln.png</v>
+      </c>
+      <c r="AU27" t="str">
+        <v>2025-03-29T07:00:07.487Z</v>
+      </c>
+      <c r="AV27" t="str">
+        <v>TEst</v>
+      </c>
+      <c r="AW27" t="str">
+        <v>609</v>
+      </c>
+      <c r="AX27" t="str">
+        <v>2025-03-29T07:00:07.487Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AX26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AX27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Taxanomy brands and other fields crud operations accomplished
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX27"/>
+  <dimension ref="A1:AX25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -566,10 +566,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <v>Dom Pérignon Vintage Champagne2</v>
+        <v>Dom Pérignon Vintage Champagne3</v>
       </c>
       <c r="D2" t="str">
-        <v>Dom Pérignon Vintage Champagne2</v>
+        <v>Dom Pérignon Vintage Champagne3</v>
       </c>
       <c r="E2" t="str">
         <v>Elegant and luxurious, Dom Pérignon is a testament to the finest in champagne making, with vibrant notes of almond, citrus, and toasted brioche.</v>
@@ -599,7 +599,7 @@
         <v>DOM PÉRIGNON</v>
       </c>
       <c r="N2" t="str">
-        <v>test2</v>
+        <v>France</v>
       </c>
       <c r="O2" t="str">
         <v>FRANCE</v>
@@ -698,7 +698,7 @@
         <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="AU2" t="str">
-        <v>2025-03-29T06:55:47.797Z</v>
+        <v>2025-03-29T07:26:26.162Z</v>
       </c>
       <c r="AV2" t="str">
         <v>wine</v>
@@ -712,10 +712,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <v>Macallan Rare Cask Single Malt</v>
+        <v>Macallan Rare Cask Single Malt2</v>
       </c>
       <c r="D3" t="str">
-        <v>Macallan Rare Cask Single Malt</v>
+        <v>Macallan Rare Cask Single Malt2</v>
       </c>
       <c r="E3" t="str">
         <v>Drawn from the broadest spectrum of casks, Rare Cask showcases the diversity of oak types and sizes that The Macallan uses to mature its whisky.</v>
@@ -790,7 +790,7 @@
         <v>750ml</v>
       </c>
       <c r="AC3" t="str">
-        <v>750 ML</v>
+        <v>750ML</v>
       </c>
       <c r="AD3" t="str">
         <v>1 x 750 ML</v>
@@ -844,7 +844,7 @@
         <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
       </c>
       <c r="AU3" t="str">
-        <v>2025-03-28T15:21:02.207Z</v>
+        <v>2025-03-29T07:36:19.940Z</v>
       </c>
       <c r="AV3" t="str">
         <v>SPIRITS</v>
@@ -2538,10 +2538,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="str">
-        <v>Casamigos Blanco Tequila</v>
+        <v>Casamigos Blanco Tequila3</v>
       </c>
       <c r="D16" t="str">
-        <v>Casamigos Blanco Tequila</v>
+        <v>Casamigos Blanco Tequila3</v>
       </c>
       <c r="E16" t="str">
         <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
@@ -2597,26 +2597,26 @@
       <c r="V16" t="str">
         <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
       </c>
-      <c r="W16" t="b">
-        <v>1</v>
-      </c>
-      <c r="X16" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA16" t="str">
-        <v>40%</v>
+      <c r="W16" t="str">
+        <v>true</v>
+      </c>
+      <c r="X16" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y16" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z16" t="str">
+        <v>true</v>
+      </c>
+      <c r="AA16">
+        <v>40</v>
       </c>
       <c r="AB16" t="str">
         <v>750ml</v>
       </c>
       <c r="AC16" t="str">
-        <v>750 ML</v>
+        <v>750ML</v>
       </c>
       <c r="AD16" t="str">
         <v>1 x 750 ML</v>
@@ -2663,8 +2663,14 @@
       <c r="AR16" t="str">
         <v/>
       </c>
-      <c r="AS16" t="b">
-        <v>1</v>
+      <c r="AS16" t="str">
+        <v>true</v>
+      </c>
+      <c r="AT16" t="str">
+        <v>https://ext.same-assets.com/1701767421/1355704146.jpeg</v>
+      </c>
+      <c r="AU16" t="str">
+        <v>2025-03-29T08:15:38.675Z</v>
       </c>
       <c r="AV16" t="str">
         <v>SPIRITS</v>
@@ -3562,205 +3568,9 @@
         <v>test category</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>608</v>
-      </c>
-      <c r="B26" t="str">
-        <v>SKU-608-717</v>
-      </c>
-      <c r="C26" t="str">
-        <v>test product</v>
-      </c>
-      <c r="D26" t="str">
-        <v>test product</v>
-      </c>
-      <c r="F26" t="str">
-        <v>beer</v>
-      </c>
-      <c r="G26" t="str">
-        <v>whiskey</v>
-      </c>
-      <c r="Q26">
-        <v>34</v>
-      </c>
-      <c r="S26">
-        <v>34</v>
-      </c>
-      <c r="T26" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743226484/vzcjhlpqnvz4i0x2uw1j.svg</v>
-      </c>
-      <c r="W26" t="str">
-        <v>false</v>
-      </c>
-      <c r="X26" t="str">
-        <v>false</v>
-      </c>
-      <c r="Y26" t="str">
-        <v>false</v>
-      </c>
-      <c r="Z26" t="str">
-        <v>false</v>
-      </c>
-      <c r="AB26" t="str">
-        <v>45ml</v>
-      </c>
-      <c r="AC26" t="str">
-        <v>45ML</v>
-      </c>
-      <c r="AG26">
-        <v>34</v>
-      </c>
-      <c r="AK26" t="str">
-        <v>taxable</v>
-      </c>
-      <c r="AL26" t="str">
-        <v>no</v>
-      </c>
-      <c r="AM26" t="str">
-        <v>no</v>
-      </c>
-      <c r="AN26" t="str">
-        <v>instock</v>
-      </c>
-      <c r="AP26" t="str">
-        <v>publish</v>
-      </c>
-      <c r="AQ26" t="str">
-        <v>open</v>
-      </c>
-      <c r="AS26" t="str">
-        <v>false</v>
-      </c>
-      <c r="AT26" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743226484/vzcjhlpqnvz4i0x2uw1j.svg</v>
-      </c>
-      <c r="AU26" t="str">
-        <v>2025-03-29T05:34:46.251Z</v>
-      </c>
-      <c r="AV26" t="str">
-        <v>beer</v>
-      </c>
-      <c r="AW26" t="str">
-        <v>608</v>
-      </c>
-      <c r="AX26" t="str">
-        <v>2025-03-29T05:34:46.251Z</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>609</v>
-      </c>
-      <c r="B27" t="str">
-        <v>SKU-609-858</v>
-      </c>
-      <c r="C27" t="str">
-        <v>category, brand  , country and varietal</v>
-      </c>
-      <c r="D27" t="str">
-        <v>category, brand  , country and varietal</v>
-      </c>
-      <c r="E27" t="str">
-        <v>category, brand  , country and varietal</v>
-      </c>
-      <c r="F27" t="str">
-        <v>TEst</v>
-      </c>
-      <c r="G27" t="str">
-        <v>test2</v>
-      </c>
-      <c r="H27" t="str">
-        <v>test2</v>
-      </c>
-      <c r="J27" t="str">
-        <v>test2</v>
-      </c>
-      <c r="L27" t="str">
-        <v>test2</v>
-      </c>
-      <c r="M27" t="str">
-        <v>test2</v>
-      </c>
-      <c r="N27" t="str">
-        <v>test2</v>
-      </c>
-      <c r="Q27">
-        <v>123</v>
-      </c>
-      <c r="S27">
-        <v>123</v>
-      </c>
-      <c r="T27" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743231607/kds3tizmge75ujw5kqln.png</v>
-      </c>
-      <c r="V27" t="str">
-        <v>category, brand  , country and varietal</v>
-      </c>
-      <c r="W27" t="str">
-        <v>false</v>
-      </c>
-      <c r="X27" t="str">
-        <v>false</v>
-      </c>
-      <c r="Y27" t="str">
-        <v>false</v>
-      </c>
-      <c r="Z27" t="str">
-        <v>false</v>
-      </c>
-      <c r="AB27" t="str">
-        <v>45ml</v>
-      </c>
-      <c r="AC27" t="str">
-        <v>45ML</v>
-      </c>
-      <c r="AG27">
-        <v>123</v>
-      </c>
-      <c r="AI27" t="str">
-        <v>test2</v>
-      </c>
-      <c r="AK27" t="str">
-        <v>taxable</v>
-      </c>
-      <c r="AL27" t="str">
-        <v>no</v>
-      </c>
-      <c r="AM27" t="str">
-        <v>no</v>
-      </c>
-      <c r="AN27" t="str">
-        <v>instock</v>
-      </c>
-      <c r="AP27" t="str">
-        <v>publish</v>
-      </c>
-      <c r="AQ27" t="str">
-        <v>open</v>
-      </c>
-      <c r="AS27" t="str">
-        <v>false</v>
-      </c>
-      <c r="AT27" t="str">
-        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743231607/kds3tizmge75ujw5kqln.png</v>
-      </c>
-      <c r="AU27" t="str">
-        <v>2025-03-29T07:00:07.487Z</v>
-      </c>
-      <c r="AV27" t="str">
-        <v>TEst</v>
-      </c>
-      <c r="AW27" t="str">
-        <v>609</v>
-      </c>
-      <c r="AX27" t="str">
-        <v>2025-03-29T07:00:07.487Z</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AX27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AX25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
User and admin authentication through cookies
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX25"/>
+  <dimension ref="A1:AX27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -566,10 +566,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <v>Dom Pérignon Vintage Champagne3</v>
+        <v>Dom Pérignon Vintage Champagne4</v>
       </c>
       <c r="D2" t="str">
-        <v>Dom Pérignon Vintage Champagne3</v>
+        <v>Dom Pérignon Vintage Champagne4</v>
       </c>
       <c r="E2" t="str">
         <v>Elegant and luxurious, Dom Pérignon is a testament to the finest in champagne making, with vibrant notes of almond, citrus, and toasted brioche.</v>
@@ -698,7 +698,7 @@
         <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="AU2" t="str">
-        <v>2025-03-29T07:26:26.162Z</v>
+        <v>2025-03-29T09:07:10.002Z</v>
       </c>
       <c r="AV2" t="str">
         <v>wine</v>
@@ -712,10 +712,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <v>Macallan Rare Cask Single Malt2</v>
+        <v>Macallan Rare Cask Single Malt</v>
       </c>
       <c r="D3" t="str">
-        <v>Macallan Rare Cask Single Malt2</v>
+        <v>Macallan Rare Cask Single Malt</v>
       </c>
       <c r="E3" t="str">
         <v>Drawn from the broadest spectrum of casks, Rare Cask showcases the diversity of oak types and sizes that The Macallan uses to mature its whisky.</v>
@@ -790,7 +790,7 @@
         <v>750ml</v>
       </c>
       <c r="AC3" t="str">
-        <v>750ML</v>
+        <v>750 ML</v>
       </c>
       <c r="AD3" t="str">
         <v>1 x 750 ML</v>
@@ -844,7 +844,7 @@
         <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
       </c>
       <c r="AU3" t="str">
-        <v>2025-03-29T07:36:19.940Z</v>
+        <v>2025-03-28T15:21:02.207Z</v>
       </c>
       <c r="AV3" t="str">
         <v>SPIRITS</v>
@@ -2538,10 +2538,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="str">
-        <v>Casamigos Blanco Tequila3</v>
+        <v>Casamigos Blanco Tequila</v>
       </c>
       <c r="D16" t="str">
-        <v>Casamigos Blanco Tequila3</v>
+        <v>Casamigos Blanco Tequila</v>
       </c>
       <c r="E16" t="str">
         <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
@@ -2597,26 +2597,26 @@
       <c r="V16" t="str">
         <v>Made from 100% Blue Weber Agave, Casamigos Blanco offers a clean, crisp taste with hints of citrus, vanilla and sweet agave.</v>
       </c>
-      <c r="W16" t="str">
-        <v>true</v>
-      </c>
-      <c r="X16" t="str">
-        <v>false</v>
-      </c>
-      <c r="Y16" t="str">
-        <v>false</v>
-      </c>
-      <c r="Z16" t="str">
-        <v>true</v>
-      </c>
-      <c r="AA16">
-        <v>40</v>
+      <c r="W16" t="b">
+        <v>1</v>
+      </c>
+      <c r="X16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="str">
+        <v>40%</v>
       </c>
       <c r="AB16" t="str">
         <v>750ml</v>
       </c>
       <c r="AC16" t="str">
-        <v>750ML</v>
+        <v>750 ML</v>
       </c>
       <c r="AD16" t="str">
         <v>1 x 750 ML</v>
@@ -2663,14 +2663,8 @@
       <c r="AR16" t="str">
         <v/>
       </c>
-      <c r="AS16" t="str">
-        <v>true</v>
-      </c>
-      <c r="AT16" t="str">
-        <v>https://ext.same-assets.com/1701767421/1355704146.jpeg</v>
-      </c>
-      <c r="AU16" t="str">
-        <v>2025-03-29T08:15:38.675Z</v>
+      <c r="AS16" t="b">
+        <v>1</v>
       </c>
       <c r="AV16" t="str">
         <v>SPIRITS</v>
@@ -3568,9 +3562,190 @@
         <v>test category</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>608</v>
+      </c>
+      <c r="B26" t="str">
+        <v>SKU-608-717</v>
+      </c>
+      <c r="C26" t="str">
+        <v>test product</v>
+      </c>
+      <c r="D26" t="str">
+        <v>test product</v>
+      </c>
+      <c r="F26" t="str">
+        <v>beer</v>
+      </c>
+      <c r="G26" t="str">
+        <v>whiskey</v>
+      </c>
+      <c r="Q26">
+        <v>34</v>
+      </c>
+      <c r="S26">
+        <v>34</v>
+      </c>
+      <c r="T26" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743226484/vzcjhlpqnvz4i0x2uw1j.svg</v>
+      </c>
+      <c r="W26" t="str">
+        <v>false</v>
+      </c>
+      <c r="X26" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y26" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z26" t="str">
+        <v>false</v>
+      </c>
+      <c r="AB26" t="str">
+        <v>45ml</v>
+      </c>
+      <c r="AC26" t="str">
+        <v>45ML</v>
+      </c>
+      <c r="AG26">
+        <v>34</v>
+      </c>
+      <c r="AK26" t="str">
+        <v>taxable</v>
+      </c>
+      <c r="AL26" t="str">
+        <v>no</v>
+      </c>
+      <c r="AM26" t="str">
+        <v>no</v>
+      </c>
+      <c r="AN26" t="str">
+        <v>instock</v>
+      </c>
+      <c r="AP26" t="str">
+        <v>publish</v>
+      </c>
+      <c r="AQ26" t="str">
+        <v>open</v>
+      </c>
+      <c r="AS26" t="str">
+        <v>false</v>
+      </c>
+      <c r="AT26" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743226484/vzcjhlpqnvz4i0x2uw1j.svg</v>
+      </c>
+      <c r="AU26" t="str">
+        <v>2025-03-29T05:34:46.251Z</v>
+      </c>
+      <c r="AV26" t="str">
+        <v>beer</v>
+      </c>
+      <c r="AW26" t="str">
+        <v>608</v>
+      </c>
+      <c r="AX26" t="str">
+        <v>2025-03-29T05:34:46.251Z</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>609</v>
+      </c>
+      <c r="B27" t="str">
+        <v>SKU-609-342</v>
+      </c>
+      <c r="C27" t="str">
+        <v>waefds</v>
+      </c>
+      <c r="D27" t="str">
+        <v>waefds</v>
+      </c>
+      <c r="F27" t="str">
+        <v>test category 34</v>
+      </c>
+      <c r="G27" t="str">
+        <v>test</v>
+      </c>
+      <c r="H27" t="str">
+        <v>test</v>
+      </c>
+      <c r="N27" t="str">
+        <v>test</v>
+      </c>
+      <c r="Q27">
+        <v>25</v>
+      </c>
+      <c r="S27">
+        <v>25</v>
+      </c>
+      <c r="T27" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743239260/awsdfs6a1sfgwh2b3ik6.jpg</v>
+      </c>
+      <c r="W27" t="str">
+        <v>false</v>
+      </c>
+      <c r="X27" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y27" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z27" t="str">
+        <v>false</v>
+      </c>
+      <c r="AB27" t="str">
+        <v>ml</v>
+      </c>
+      <c r="AC27" t="str">
+        <v>ML</v>
+      </c>
+      <c r="AG27">
+        <v>23</v>
+      </c>
+      <c r="AI27" t="str">
+        <v>test</v>
+      </c>
+      <c r="AK27" t="str">
+        <v>taxable</v>
+      </c>
+      <c r="AL27" t="str">
+        <v>no</v>
+      </c>
+      <c r="AM27" t="str">
+        <v>no</v>
+      </c>
+      <c r="AN27" t="str">
+        <v>instock</v>
+      </c>
+      <c r="AP27" t="str">
+        <v>publish</v>
+      </c>
+      <c r="AQ27" t="str">
+        <v>open</v>
+      </c>
+      <c r="AS27" t="str">
+        <v>false</v>
+      </c>
+      <c r="AT27" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743239260/awsdfs6a1sfgwh2b3ik6.jpg</v>
+      </c>
+      <c r="AU27" t="str">
+        <v>2025-03-29T09:07:41.265Z</v>
+      </c>
+      <c r="AV27" t="str">
+        <v>test category 34</v>
+      </c>
+      <c r="AW27" t="str">
+        <v>609</v>
+      </c>
+      <c r="AX27" t="str">
+        <v>2025-03-29T09:07:41.265Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AX25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AX27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
User and admin authentication created using google
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -566,10 +566,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <v>Dom Pérignon Vintage Champagne4</v>
+        <v>Dom Pérignon Vintage Champagne6</v>
       </c>
       <c r="D2" t="str">
-        <v>Dom Pérignon Vintage Champagne4</v>
+        <v>Dom Pérignon Vintage Champagne6</v>
       </c>
       <c r="E2" t="str">
         <v>Elegant and luxurious, Dom Pérignon is a testament to the finest in champagne making, with vibrant notes of almond, citrus, and toasted brioche.</v>
@@ -641,10 +641,10 @@
         <v>12.5</v>
       </c>
       <c r="AB2" t="str">
-        <v>750ml</v>
+        <v>758ml</v>
       </c>
       <c r="AC2" t="str">
-        <v>750ML</v>
+        <v>758ML</v>
       </c>
       <c r="AD2" t="str">
         <v>1 x 750 ML</v>
@@ -698,7 +698,7 @@
         <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="AU2" t="str">
-        <v>2025-03-29T09:07:10.002Z</v>
+        <v>2025-03-29T18:20:23.371Z</v>
       </c>
       <c r="AV2" t="str">
         <v>wine</v>

</xml_diff>

<commit_message>
Admin can see and change order status and notification goes to user in real time
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -1698,10 +1698,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="str">
-        <v>Caymus Cabernet Sauvignon</v>
+        <v>Caymus Cabernet Sauvignon2</v>
       </c>
       <c r="D10" t="str">
-        <v>Caymus Cabernet Sauvignon</v>
+        <v>Caymus Cabernet Sauvignon2</v>
       </c>
       <c r="E10" t="str">
         <v>A rich, deeply colored and concentrated Cabernet from Napa Valley with scents of dark berries, currants and sweet vanilla oak.</v>
@@ -1757,26 +1757,26 @@
       <c r="V10" t="str">
         <v>A rich, deeply colored and concentrated Cabernet from Napa Valley with scents of dark berries, currants and sweet vanilla oak.</v>
       </c>
-      <c r="W10" t="b">
-        <v>0</v>
-      </c>
-      <c r="X10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y10" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA10" t="str">
-        <v>14.6%</v>
+      <c r="W10" t="str">
+        <v>false</v>
+      </c>
+      <c r="X10" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y10" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z10" t="str">
+        <v>true</v>
+      </c>
+      <c r="AA10">
+        <v>14.6</v>
       </c>
       <c r="AB10" t="str">
-        <v>750ml</v>
+        <v>75ml</v>
       </c>
       <c r="AC10" t="str">
-        <v>750 ML</v>
+        <v>75ML</v>
       </c>
       <c r="AD10" t="str">
         <v>1 x 750 ML</v>
@@ -1823,8 +1823,14 @@
       <c r="AR10" t="str">
         <v>RED</v>
       </c>
-      <c r="AS10" t="b">
-        <v>1</v>
+      <c r="AS10" t="str">
+        <v>true</v>
+      </c>
+      <c r="AT10" t="str">
+        <v>https://ext.same-assets.com/1701767421/4224202088.png</v>
+      </c>
+      <c r="AU10" t="str">
+        <v>2025-03-30T18:18:14.916Z</v>
       </c>
       <c r="AV10" t="str">
         <v>WINE</v>
@@ -1978,10 +1984,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="str">
-        <v>Corona Extra</v>
+        <v>Corona Extra45</v>
       </c>
       <c r="D12" t="str">
-        <v>Corona Extra</v>
+        <v>Corona Extra45</v>
       </c>
       <c r="E12" t="str">
         <v>A light, crisp and refreshing beer with a hint of fruity-honey aroma. Perfect with a wedge of lime on a hot day.</v>
@@ -2037,26 +2043,26 @@
       <c r="V12" t="str">
         <v>A light, crisp and refreshing beer with a hint of fruity-honey aroma. Perfect with a wedge of lime on a hot day.</v>
       </c>
-      <c r="W12" t="b">
-        <v>0</v>
-      </c>
-      <c r="X12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA12" t="str">
-        <v>4.5%</v>
+      <c r="W12" t="str">
+        <v>false</v>
+      </c>
+      <c r="X12" t="str">
+        <v>false</v>
+      </c>
+      <c r="Y12" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z12" t="str">
+        <v>false</v>
+      </c>
+      <c r="AA12">
+        <v>4.5</v>
       </c>
       <c r="AB12" t="str">
-        <v>6 pack - 330ml</v>
+        <v>633ml</v>
       </c>
       <c r="AC12" t="str">
-        <v>6 pack - 330 ML</v>
+        <v>633ML</v>
       </c>
       <c r="AD12" t="str">
         <v>1 x 6 pack - 330 ML</v>
@@ -2103,8 +2109,14 @@
       <c r="AR12" t="str">
         <v/>
       </c>
-      <c r="AS12" t="b">
-        <v>1</v>
+      <c r="AS12" t="str">
+        <v>true</v>
+      </c>
+      <c r="AT12" t="str">
+        <v>https://ext.same-assets.com/1701767421/2183896642.jpeg</v>
+      </c>
+      <c r="AU12" t="str">
+        <v>2025-03-30T18:17:12.776Z</v>
       </c>
       <c r="AV12" t="str">
         <v>BEER</v>

</xml_diff>

<commit_message>
Added stock update through socket io problem fixed
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX27"/>
+  <dimension ref="A1:AY27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -552,9 +552,12 @@
         <v>tax:product_cat</v>
       </c>
       <c r="AW1" t="str">
+        <v>stock_quantity</v>
+      </c>
+      <c r="AX1" t="str">
         <v>ID</v>
       </c>
-      <c r="AX1" t="str">
+      <c r="AY1" t="str">
         <v>date_created</v>
       </c>
     </row>
@@ -641,10 +644,10 @@
         <v>12.5</v>
       </c>
       <c r="AB2" t="str">
-        <v>758ml</v>
+        <v>7ml</v>
       </c>
       <c r="AC2" t="str">
-        <v>758ML</v>
+        <v>7ML</v>
       </c>
       <c r="AD2" t="str">
         <v>1 x 750 ML</v>
@@ -656,7 +659,7 @@
         <v>3 LB</v>
       </c>
       <c r="AG2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AH2" t="str">
         <v>featured</v>
@@ -698,10 +701,13 @@
         <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="AU2" t="str">
-        <v>2025-03-29T18:20:23.371Z</v>
+        <v>2025-03-31T17:11:56.419Z</v>
       </c>
       <c r="AV2" t="str">
         <v>wine</v>
+      </c>
+      <c r="AW2">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -724,10 +730,10 @@
         <v>spirits</v>
       </c>
       <c r="G3" t="str">
-        <v>scotch</v>
+        <v>vodka</v>
       </c>
       <c r="H3" t="str">
-        <v>SCOTCH</v>
+        <v>vodka</v>
       </c>
       <c r="I3" t="str">
         <v xml:space="preserve">SCOTCH  </v>
@@ -787,10 +793,10 @@
         <v>43</v>
       </c>
       <c r="AB3" t="str">
-        <v>750ml</v>
+        <v>75ml</v>
       </c>
       <c r="AC3" t="str">
-        <v>750 ML</v>
+        <v>75ML</v>
       </c>
       <c r="AD3" t="str">
         <v>1 x 750 ML</v>
@@ -808,7 +814,7 @@
         <v>featured</v>
       </c>
       <c r="AI3" t="str">
-        <v>simple</v>
+        <v>vodka</v>
       </c>
       <c r="AJ3" t="str">
         <v>yes</v>
@@ -844,10 +850,13 @@
         <v>https://ext.same-assets.com/1701767421/2633843034.png</v>
       </c>
       <c r="AU3" t="str">
-        <v>2025-03-28T15:21:02.207Z</v>
+        <v>2025-03-31T17:01:46.261Z</v>
       </c>
       <c r="AV3" t="str">
         <v>SPIRITS</v>
+      </c>
+      <c r="AW3">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -989,6 +998,9 @@
       <c r="AV4" t="str">
         <v>WINE</v>
       </c>
+      <c r="AW4">
+        <v>32</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -1129,6 +1141,9 @@
       <c r="AV5" t="str">
         <v>SPIRITS</v>
       </c>
+      <c r="AW5">
+        <v>34</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -1269,6 +1284,9 @@
       <c r="AV6" t="str">
         <v>SPIRITS</v>
       </c>
+      <c r="AW6">
+        <v>45</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -1409,6 +1427,9 @@
       <c r="AV7" t="str">
         <v>SPIRITS</v>
       </c>
+      <c r="AW7">
+        <v>45</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -1549,6 +1570,9 @@
       <c r="AV8" t="str">
         <v>SPIRITS</v>
       </c>
+      <c r="AW8">
+        <v>65</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -1689,6 +1713,9 @@
       <c r="AV9" t="str">
         <v>SPIRITS</v>
       </c>
+      <c r="AW9">
+        <v>65</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -1835,6 +1862,9 @@
       <c r="AV10" t="str">
         <v>WINE</v>
       </c>
+      <c r="AW10">
+        <v>66</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -1975,6 +2005,9 @@
       <c r="AV11" t="str">
         <v>WINE</v>
       </c>
+      <c r="AW11">
+        <v>66</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -2059,10 +2092,10 @@
         <v>4.5</v>
       </c>
       <c r="AB12" t="str">
-        <v>633ml</v>
+        <v>63ml</v>
       </c>
       <c r="AC12" t="str">
-        <v>633ML</v>
+        <v>63ML</v>
       </c>
       <c r="AD12" t="str">
         <v>1 x 6 pack - 330 ML</v>
@@ -2074,7 +2107,7 @@
         <v>3 LB</v>
       </c>
       <c r="AG12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AH12" t="str">
         <v>visible</v>
@@ -2116,10 +2149,13 @@
         <v>https://ext.same-assets.com/1701767421/2183896642.jpeg</v>
       </c>
       <c r="AU12" t="str">
-        <v>2025-03-30T18:17:12.776Z</v>
+        <v>2025-03-31T17:08:09.075Z</v>
       </c>
       <c r="AV12" t="str">
         <v>BEER</v>
+      </c>
+      <c r="AW12">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -2261,6 +2297,9 @@
       <c r="AV13" t="str">
         <v>BEER</v>
       </c>
+      <c r="AW13">
+        <v>6</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -2401,6 +2440,9 @@
       <c r="AV14" t="str">
         <v>BEER</v>
       </c>
+      <c r="AW14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -2541,6 +2583,9 @@
       <c r="AV15" t="str">
         <v>BEER</v>
       </c>
+      <c r="AW15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -2681,6 +2726,9 @@
       <c r="AV16" t="str">
         <v>SPIRITS</v>
       </c>
+      <c r="AW16">
+        <v>45</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -2821,6 +2869,9 @@
       <c r="AV17" t="str">
         <v>WINE</v>
       </c>
+      <c r="AW17">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" xml:space="preserve">
       <c r="A18" t="str">
@@ -2914,10 +2965,13 @@
       <c r="AV18" t="str">
         <v>spirits</v>
       </c>
-      <c r="AW18" t="str">
+      <c r="AW18">
+        <v>32</v>
+      </c>
+      <c r="AX18" t="str">
         <v>600</v>
       </c>
-      <c r="AX18" t="str">
+      <c r="AY18" t="str">
         <v>2025-03-28T12:17:35.575Z</v>
       </c>
     </row>
@@ -3018,10 +3072,13 @@
       <c r="AV19" t="str">
         <v>wine</v>
       </c>
-      <c r="AW19" t="str">
+      <c r="AW19">
+        <v>2</v>
+      </c>
+      <c r="AX19" t="str">
         <v>601</v>
       </c>
-      <c r="AX19" t="str">
+      <c r="AY19" t="str">
         <v>2025-03-28T12:25:00.293Z</v>
       </c>
     </row>
@@ -3116,10 +3173,13 @@
       <c r="AV20" t="str">
         <v>beer</v>
       </c>
-      <c r="AW20" t="str">
+      <c r="AW20">
+        <v>3</v>
+      </c>
+      <c r="AX20" t="str">
         <v>602</v>
       </c>
-      <c r="AX20" t="str">
+      <c r="AY20" t="str">
         <v>2025-03-28T12:31:41.045Z</v>
       </c>
     </row>
@@ -3214,10 +3274,13 @@
       <c r="AV21" t="str">
         <v>wine</v>
       </c>
-      <c r="AW21" t="str">
+      <c r="AW21">
+        <v>4</v>
+      </c>
+      <c r="AX21" t="str">
         <v>603</v>
       </c>
-      <c r="AX21" t="str">
+      <c r="AY21" t="str">
         <v>2025-03-28T12:46:29.945Z</v>
       </c>
     </row>
@@ -3315,10 +3378,13 @@
       <c r="AV22" t="str">
         <v>wine</v>
       </c>
-      <c r="AW22" t="str">
+      <c r="AW22">
+        <v>5</v>
+      </c>
+      <c r="AX22" t="str">
         <v>604</v>
       </c>
-      <c r="AX22" t="str">
+      <c r="AY22" t="str">
         <v>2025-03-28T13:16:01.109Z</v>
       </c>
     </row>
@@ -3410,10 +3476,13 @@
       <c r="AV23" t="str">
         <v>wine</v>
       </c>
-      <c r="AW23" t="str">
+      <c r="AW23">
+        <v>6</v>
+      </c>
+      <c r="AX23" t="str">
         <v>605</v>
       </c>
-      <c r="AX23" t="str">
+      <c r="AY23" t="str">
         <v>2025-03-28T14:45:57.115Z</v>
       </c>
     </row>
@@ -3496,10 +3565,13 @@
       <c r="AV24" t="str">
         <v>spirits</v>
       </c>
-      <c r="AW24" t="str">
+      <c r="AW24">
+        <v>7</v>
+      </c>
+      <c r="AX24" t="str">
         <v>606</v>
       </c>
-      <c r="AX24" t="str">
+      <c r="AY24" t="str">
         <v>2025-03-28T15:15:57.426Z</v>
       </c>
     </row>
@@ -3573,6 +3645,9 @@
       <c r="AV25" t="str">
         <v>test category</v>
       </c>
+      <c r="AW25">
+        <v>6</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -3653,10 +3728,13 @@
       <c r="AV26" t="str">
         <v>beer</v>
       </c>
-      <c r="AW26" t="str">
+      <c r="AW26">
+        <v>7</v>
+      </c>
+      <c r="AX26" t="str">
         <v>608</v>
       </c>
-      <c r="AX26" t="str">
+      <c r="AY26" t="str">
         <v>2025-03-29T05:34:46.251Z</v>
       </c>
     </row>
@@ -3748,16 +3826,19 @@
       <c r="AV27" t="str">
         <v>test category 34</v>
       </c>
-      <c r="AW27" t="str">
+      <c r="AW27">
+        <v>9</v>
+      </c>
+      <c r="AX27" t="str">
         <v>609</v>
       </c>
-      <c r="AX27" t="str">
+      <c r="AY27" t="str">
         <v>2025-03-29T09:07:41.265Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AX27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AY27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Stock push notification to admin left
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -644,10 +644,10 @@
         <v>12.5</v>
       </c>
       <c r="AB2" t="str">
-        <v>7ml</v>
+        <v>4ml</v>
       </c>
       <c r="AC2" t="str">
-        <v>7ML</v>
+        <v>4ML</v>
       </c>
       <c r="AD2" t="str">
         <v>1 x 750 ML</v>
@@ -659,7 +659,7 @@
         <v>3 LB</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2" t="str">
         <v>featured</v>
@@ -680,7 +680,7 @@
         <v>no</v>
       </c>
       <c r="AN2" t="str">
-        <v>instock</v>
+        <v>outofstock</v>
       </c>
       <c r="AO2" t="str">
         <v>visible</v>
@@ -701,13 +701,13 @@
         <v>https://ext.same-assets.com/1701767421/2884727806.png</v>
       </c>
       <c r="AU2" t="str">
-        <v>2025-03-31T17:11:56.419Z</v>
+        <v>2025-03-31T17:46:46.219Z</v>
       </c>
       <c r="AV2" t="str">
         <v>wine</v>
       </c>
       <c r="AW2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
fixed admin dashboard issues
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY27"/>
+  <dimension ref="A1:AY28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3836,9 +3836,113 @@
         <v>2025-03-29T09:07:41.265Z</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>610</v>
+      </c>
+      <c r="B28" t="str">
+        <v>SKU-610-556</v>
+      </c>
+      <c r="C28" t="str">
+        <v>new</v>
+      </c>
+      <c r="D28" t="str">
+        <v>new</v>
+      </c>
+      <c r="F28" t="str">
+        <v>new</v>
+      </c>
+      <c r="G28" t="str">
+        <v>new</v>
+      </c>
+      <c r="H28" t="str">
+        <v>new</v>
+      </c>
+      <c r="L28" t="str">
+        <v>new</v>
+      </c>
+      <c r="M28" t="str">
+        <v>new</v>
+      </c>
+      <c r="N28" t="str">
+        <v>new</v>
+      </c>
+      <c r="Q28">
+        <v>23</v>
+      </c>
+      <c r="S28">
+        <v>23</v>
+      </c>
+      <c r="T28" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743509747/bk6ju4wqhoysv2yy19bd.png</v>
+      </c>
+      <c r="W28" t="str">
+        <v>false</v>
+      </c>
+      <c r="X28" t="str">
+        <v>true</v>
+      </c>
+      <c r="Y28" t="str">
+        <v>false</v>
+      </c>
+      <c r="Z28" t="str">
+        <v>false</v>
+      </c>
+      <c r="AB28" t="str">
+        <v>11ml</v>
+      </c>
+      <c r="AC28" t="str">
+        <v>11ML</v>
+      </c>
+      <c r="AG28">
+        <v>23</v>
+      </c>
+      <c r="AI28" t="str">
+        <v>new</v>
+      </c>
+      <c r="AK28" t="str">
+        <v>taxable</v>
+      </c>
+      <c r="AL28" t="str">
+        <v>no</v>
+      </c>
+      <c r="AM28" t="str">
+        <v>no</v>
+      </c>
+      <c r="AN28" t="str">
+        <v>instock</v>
+      </c>
+      <c r="AP28" t="str">
+        <v>publish</v>
+      </c>
+      <c r="AQ28" t="str">
+        <v>open</v>
+      </c>
+      <c r="AS28" t="str">
+        <v>false</v>
+      </c>
+      <c r="AT28" t="str">
+        <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743509747/bk6ju4wqhoysv2yy19bd.png</v>
+      </c>
+      <c r="AU28" t="str">
+        <v>2025-04-01T12:15:47.737Z</v>
+      </c>
+      <c r="AV28" t="str">
+        <v>new</v>
+      </c>
+      <c r="AW28">
+        <v>23</v>
+      </c>
+      <c r="AX28" t="str">
+        <v>610</v>
+      </c>
+      <c r="AY28" t="str">
+        <v>2025-04-01T12:15:47.737Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AY27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AY28"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filtering through navbar unchecking issue fixed
</commit_message>
<xml_diff>
--- a/server/public/products.xlsx
+++ b/server/public/products.xlsx
@@ -3844,10 +3844,10 @@
         <v>SKU-610-556</v>
       </c>
       <c r="C28" t="str">
-        <v>new</v>
+        <v>new6</v>
       </c>
       <c r="D28" t="str">
-        <v>new</v>
+        <v>new6</v>
       </c>
       <c r="F28" t="str">
         <v>new</v>
@@ -3867,6 +3867,9 @@
       <c r="N28" t="str">
         <v>new</v>
       </c>
+      <c r="O28" t="str">
+        <v>new</v>
+      </c>
       <c r="Q28">
         <v>23</v>
       </c>
@@ -3889,13 +3892,13 @@
         <v>false</v>
       </c>
       <c r="AB28" t="str">
-        <v>11ml</v>
+        <v>23ml</v>
       </c>
       <c r="AC28" t="str">
-        <v>11ML</v>
+        <v>23ML</v>
       </c>
       <c r="AG28">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="AI28" t="str">
         <v>new</v>
@@ -3910,7 +3913,7 @@
         <v>no</v>
       </c>
       <c r="AN28" t="str">
-        <v>instock</v>
+        <v>outofstock</v>
       </c>
       <c r="AP28" t="str">
         <v>publish</v>
@@ -3925,13 +3928,13 @@
         <v>https://res.cloudinary.com/dc3hqcovg/image/upload/v1743509747/bk6ju4wqhoysv2yy19bd.png</v>
       </c>
       <c r="AU28" t="str">
-        <v>2025-04-01T12:15:47.737Z</v>
+        <v>2025-04-01T12:25:11.319Z</v>
       </c>
       <c r="AV28" t="str">
         <v>new</v>
       </c>
       <c r="AW28">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="AX28" t="str">
         <v>610</v>

</xml_diff>